<commit_message>
New publication, updated OS commitments
</commit_message>
<xml_diff>
--- a/research.xlsx
+++ b/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lroesele.IVV5NET\sciebo - Röseler, Lukas (lroesele@uni-muenster.de)@uni-muenster.sciebo.de\LeaRn\home\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF2A24C-04CD-450F-8317-82EE55491458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399B7169-16C3-4501-BBE8-5C881F006A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AAC91D46-EE41-4CEB-9A66-251368506452}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="135">
   <si>
     <t>#</t>
   </si>
@@ -501,6 +501,35 @@
   </si>
   <si>
     <t>Weber, L., &amp; Röseler, L. (2025). Testing the Reliability of Anchoring Susceptibility Scores. Europe’s Journal of Psychology, 21(1), 1-10. https://doi.org/10.5964/ejop.9891</t>
+  </si>
+  <si>
+    <t>Gold (APC: 2790.00€)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hoghe, J., </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Röseler, L.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Limmer, R., Walther, C., &amp; Schütz, A. (2025). Die Bedeutung personaler Ressourcen und personaler Risikofaktoren für die Bewältigung beruflicher Belastungen bei Genesungsbegleiter/-innen/Peer Berater/-innen. In Zeitschrift für Arbeitswissenschaft. https://doi.org/10.1007/s41449-025-00460-x </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -570,7 +599,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -593,6 +622,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -909,10 +944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D3A1534-13D7-4FF4-8CD6-0F369116C1B6}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,97 +983,97 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="7"/>
+      <c r="G2" s="1"/>
       <c r="H2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
+        <v>32</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>31</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="4" t="s">
+      <c r="F4" s="7"/>
+      <c r="G4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="H4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>30</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>29</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>21</v>
@@ -1046,23 +1081,23 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>123</v>
+        <v>22</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>21</v>
@@ -1070,23 +1105,23 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
+        <v>28</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>21</v>
@@ -1094,25 +1129,23 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>35</v>
+        <v>20</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>21</v>
@@ -1120,87 +1153,91 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>29</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D10" s="7"/>
       <c r="E10" s="4" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="4" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="7"/>
+        <v>29</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="G11" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="H11" s="2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>48</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="2" t="s">
         <v>10</v>
@@ -1208,63 +1245,65 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>124</v>
+        <v>50</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="G14" s="7"/>
       <c r="H14" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+        <v>52</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>124</v>
+      </c>
       <c r="G15" s="7"/>
       <c r="H15" s="2" t="s">
         <v>21</v>
@@ -1272,44 +1311,40 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>35</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>61</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="D17" s="7"/>
       <c r="E17" s="2" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="2" t="s">
@@ -1318,20 +1353,22 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" s="7"/>
+        <v>58</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="E18" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G18" s="7"/>
       <c r="H18" s="2" t="s">
@@ -1340,47 +1377,45 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>69</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="G19" s="7"/>
       <c r="H19" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="D20" s="7"/>
       <c r="E20" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F20" s="7"/>
+        <v>67</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="G20" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>10</v>
@@ -1388,25 +1423,23 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>10</v>
@@ -1414,23 +1447,25 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F22" s="7"/>
+        <v>75</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="G22" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>10</v>
@@ -1438,25 +1473,23 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>10</v>
@@ -1464,353 +1497,382 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F24" s="7"/>
+        <v>35</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="G24" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>89</v>
+      <c r="E25" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>91</v>
+        <v>22</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>35</v>
+      <c r="E26" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>125</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>94</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>132</v>
+        <v>95</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
+        <v>7</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
         <v>6</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>5</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>105</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F30" s="7"/>
+        <v>103</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="G30" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>78</v>
+        <v>33</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>127</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="F31" s="7"/>
       <c r="G31" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>128</v>
+        <v>109</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>127</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>35</v>
+        <v>112</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>117</v>
+        <v>42</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>1</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G35" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="H35" s="2" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{41A1C6B5-F794-4E36-A76C-521B33FA2C7E}"/>
-    <hyperlink ref="F2" r:id="rId2" xr:uid="{D45BBE43-E931-4EDA-AB62-49ECCD4358D7}"/>
-    <hyperlink ref="C3" r:id="rId3" display="https://doi.org/10.5281/zenodo.13945051" xr:uid="{15B1DF19-42C9-4721-BDEE-790C2BD36401}"/>
-    <hyperlink ref="E3" r:id="rId4" xr:uid="{EE424F71-99CE-4EE2-B51B-A911BE1F8393}"/>
-    <hyperlink ref="G3" r:id="rId5" xr:uid="{3F25FBC9-AB32-4C97-9E08-65B039840DB8}"/>
-    <hyperlink ref="C4" r:id="rId6" display="https://doi.org/10.18718/81781.38" xr:uid="{782B69DE-8E85-4D8F-9DAC-8EB607F3F04E}"/>
-    <hyperlink ref="E4" r:id="rId7" xr:uid="{9A588C41-B2AF-4BF7-9A00-6DD9FB5CABFD}"/>
-    <hyperlink ref="F4" r:id="rId8" display="https://osf.io/8k9nt/" xr:uid="{159ED34F-FF9E-488E-B419-5DB75A1053A4}"/>
-    <hyperlink ref="C5" r:id="rId9" display="https://doi.org/10.15626/MP.2022.3236" xr:uid="{365B7B56-6668-4E66-B95F-686BDD31EEE7}"/>
-    <hyperlink ref="E5" r:id="rId10" xr:uid="{6F806BFE-1E43-477A-98D8-853E317AB860}"/>
-    <hyperlink ref="G5" r:id="rId11" xr:uid="{39191331-4837-4425-955D-F7F137894FA7}"/>
-    <hyperlink ref="E6" r:id="rId12" xr:uid="{BF2F029F-64B8-458D-9E6D-FB7B0A9D9E54}"/>
-    <hyperlink ref="G6" r:id="rId13" xr:uid="{130EB372-4CDB-40F4-B733-C289D48B1C4C}"/>
-    <hyperlink ref="C7" r:id="rId14" display="https://doi.org/10.15626/MP.2020.2639" xr:uid="{B96128B1-8C8B-4E74-8D94-6ECC038C9AAC}"/>
-    <hyperlink ref="E7" r:id="rId15" xr:uid="{AD4669E7-2751-41A0-BCE5-14632257828B}"/>
-    <hyperlink ref="G7" r:id="rId16" xr:uid="{3D2FC1C8-D1F7-407E-B397-D60D8B7AA2EA}"/>
-    <hyperlink ref="C8" r:id="rId17" display="https://doi.org/10.5334/jopd.92" xr:uid="{A071F59A-946C-461F-A4B7-033C6C45173A}"/>
-    <hyperlink ref="C9" r:id="rId18" display="https://doi.org/10.1016/j.jbusres.2023.114189" xr:uid="{51055E7B-DEE6-4A19-92E4-D1721DF822B1}"/>
-    <hyperlink ref="E9" r:id="rId19" xr:uid="{ED578A9E-FF99-4C7B-8A91-7C05D3B75022}"/>
-    <hyperlink ref="G9" r:id="rId20" xr:uid="{9BB5D8E7-F006-4255-8265-71EA7D3EBCE4}"/>
-    <hyperlink ref="C10" r:id="rId21" display="http://doi.org/10.5334/jopd.67" xr:uid="{C4050047-C1E1-404E-B073-E0C05CE8D173}"/>
-    <hyperlink ref="E10" r:id="rId22" xr:uid="{E3FEC74A-0F6F-4FFC-8AC0-B45670656896}"/>
-    <hyperlink ref="G10" r:id="rId23" xr:uid="{5C54A4BE-8B8C-494A-B29D-49F490A2C1C2}"/>
-    <hyperlink ref="C11" r:id="rId24" display="https://doi.org/10.1073/pnas.212037711" xr:uid="{C93D8067-4FC0-4D8D-8E47-D00FBE2F6608}"/>
-    <hyperlink ref="C12" r:id="rId25" display="https://doi.org/10.1037/bul0000356" xr:uid="{BDFC91BF-1233-4C67-A06A-DDE12D0F8BEB}"/>
-    <hyperlink ref="E12" r:id="rId26" xr:uid="{D92AA8D7-14D0-4433-B7CB-0E1DF9F275E9}"/>
-    <hyperlink ref="F12" r:id="rId27" xr:uid="{FB02A3AD-7B15-4C0E-9F16-631065DCF554}"/>
-    <hyperlink ref="C13" r:id="rId28" display="https://doi.org/10.1080/02699931.2021.1979473" xr:uid="{AD06D523-F5DB-442E-B989-A6C32B777ED1}"/>
-    <hyperlink ref="E13" r:id="rId29" xr:uid="{7BB9E6E9-A4CD-49AA-A55E-7BDA3DFBBEC0}"/>
-    <hyperlink ref="F13" r:id="rId30" xr:uid="{21E90428-3D65-4277-B80F-141F81A55916}"/>
-    <hyperlink ref="C14" r:id="rId31" display="https://doi.org/10.1016/j.jesp.2020.104066" xr:uid="{2A8C850C-91E2-46B0-987D-55EB0D9C3B0F}"/>
-    <hyperlink ref="E14" r:id="rId32" display="https://osf.io/96de2" xr:uid="{6C52A618-C82D-476C-89C8-16F20F642485}"/>
-    <hyperlink ref="C15" r:id="rId33" display="https://doi.org/10.5964/ejop.2639" xr:uid="{0DFC4B36-9C4B-4E2A-92F6-E6D628E09B18}"/>
-    <hyperlink ref="C16" r:id="rId34" display="https://doi.org/10.1177/1745691620984474" xr:uid="{54D1B1A1-B51A-4CA8-9C8A-8B2BF483FDDC}"/>
-    <hyperlink ref="C17" r:id="rId35" display="https://doi.org/10.1016/j.jesp.2020.104060" xr:uid="{862E7504-584A-4242-9B75-22375BC49E27}"/>
-    <hyperlink ref="C18" r:id="rId36" display="https://doi.org/10.1016/j.jesp.2019.103942" xr:uid="{B8F41347-13BD-4D71-A682-6BD22F709DE9}"/>
-    <hyperlink ref="C19" r:id="rId37" display="https://doi.org/10.1037/bul0000220" xr:uid="{065B9BF3-E67C-451C-B12A-2782BA816965}"/>
-    <hyperlink ref="G19" r:id="rId38" display="https://www.researchgate.net/publication/337261659_Crowdsourcing_Hypothesis_Tests_Making_Transparent_How_Design_Choices_Shape_Research_Results" xr:uid="{099DB906-00A3-4756-8332-B3B87A0D9EEF}"/>
-    <hyperlink ref="C20" r:id="rId39" display="https://osf.io/34sv6" xr:uid="{DD65BC2F-BFCE-4797-B982-DFEB045FD826}"/>
-    <hyperlink ref="G20" r:id="rId40" xr:uid="{87350DFD-AAFD-4459-9249-138523C66895}"/>
-    <hyperlink ref="C21" r:id="rId41" display="https://doi.org/10.31234/osf.io/akfzh" xr:uid="{9B39A2DF-F148-4367-8E24-E1AFFA69762A}"/>
-    <hyperlink ref="F21" r:id="rId42" xr:uid="{BACE566D-5B6D-4E9A-81EF-685F01A92950}"/>
-    <hyperlink ref="C22" r:id="rId43" display="https://doi.org/10.31234/osf.io/gj76p" xr:uid="{B34F1845-E395-44F6-9C3F-A1DC39394D59}"/>
-    <hyperlink ref="C23" r:id="rId44" display="https://doi.org/10.31234/osf.io/krwcn" xr:uid="{BEF8554E-090A-4B5A-89F1-432B57FC20C6}"/>
-    <hyperlink ref="G23" r:id="rId45" xr:uid="{5C9D188F-41F0-4255-9A7F-776DC0D7C6B3}"/>
-    <hyperlink ref="C24" r:id="rId46" display="https://osf.io/preprints/metaarxiv/ewb2t" xr:uid="{73F38CDC-AE74-42AE-9875-B80E70CAAD04}"/>
-    <hyperlink ref="G24" r:id="rId47" xr:uid="{F242B96D-FDF5-4CE7-BDFB-CFE6A00240A0}"/>
-    <hyperlink ref="C25" r:id="rId48" display="https://osf.io/8cwpy" xr:uid="{092A1365-FCB4-41FB-8313-CF735B66A2DD}"/>
-    <hyperlink ref="E25" r:id="rId49" xr:uid="{ECBA28D3-FB1C-4193-901B-41108340BCFD}"/>
-    <hyperlink ref="F25" r:id="rId50" display="https://osf.io/c2ynz" xr:uid="{E93BA08A-3A49-4D35-AC66-D74574AF96C4}"/>
-    <hyperlink ref="C27" r:id="rId51" display="https://doi.org/10.31222/osf.io/8psw2" xr:uid="{C0F54102-918A-4578-B027-C78823FD4B7D}"/>
-    <hyperlink ref="F27" r:id="rId52" xr:uid="{97ACEB9A-0C43-4AA2-ACFE-F50A4B6B56F0}"/>
-    <hyperlink ref="C28" r:id="rId53" display="https://doi.org/10.31234/osf.io/2kfh3" xr:uid="{FE4142A2-4633-4F53-8F23-5F50CB46E97C}"/>
-    <hyperlink ref="F28" r:id="rId54" xr:uid="{174B565C-80A9-4205-A2B1-E2DC35E916D7}"/>
-    <hyperlink ref="C29" r:id="rId55" display="https://doi.org/10.31234/osf.io/ntukz" xr:uid="{562912E7-E3CF-4637-A5EC-F5598C18FAED}"/>
-    <hyperlink ref="F29" r:id="rId56" display="https://osf.io/7pw4c/" xr:uid="{E5872E1A-19BD-48E3-BBC5-0325DE4F50E7}"/>
-    <hyperlink ref="C30" r:id="rId57" display="https://doi.org/10.31234/osf.io/wf2tn" xr:uid="{A453771E-19D2-48CD-8D51-59EE29E521DB}"/>
-    <hyperlink ref="C31" r:id="rId58" display="https://doi.org/10.31219/osf.io/2tr6q" xr:uid="{0F998EE8-1C6C-4120-A8A7-D2F043592BCD}"/>
-    <hyperlink ref="F31" r:id="rId59" display="https://osf.io/9qz3d" xr:uid="{4BBBB1B2-2501-4EEF-8BB3-87C7A2170367}"/>
-    <hyperlink ref="C32" r:id="rId60" display="https://doi.org/10.31234/osf.io/hjbwp" xr:uid="{519680D7-CB35-4C47-AB82-99AC96EA8DFE}"/>
-    <hyperlink ref="C33" r:id="rId61" display="https://doi.org/10.31234/osf.io/mt49r" xr:uid="{9EA40F6E-B1C1-4A75-B481-39C90A03E75E}"/>
-    <hyperlink ref="C34" r:id="rId62" display="https://doi.org/10.31234/osf.io/bnsx2" xr:uid="{63D5CDF4-C3ED-4621-886B-026265E45F56}"/>
-    <hyperlink ref="E34" r:id="rId63" xr:uid="{08AABF7C-2FA2-46EF-98CF-56A84170523F}"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{41A1C6B5-F794-4E36-A76C-521B33FA2C7E}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{D45BBE43-E931-4EDA-AB62-49ECCD4358D7}"/>
+    <hyperlink ref="C4" r:id="rId3" display="https://doi.org/10.5281/zenodo.13945051" xr:uid="{15B1DF19-42C9-4721-BDEE-790C2BD36401}"/>
+    <hyperlink ref="E4" r:id="rId4" xr:uid="{EE424F71-99CE-4EE2-B51B-A911BE1F8393}"/>
+    <hyperlink ref="G4" r:id="rId5" xr:uid="{3F25FBC9-AB32-4C97-9E08-65B039840DB8}"/>
+    <hyperlink ref="C5" r:id="rId6" display="https://doi.org/10.18718/81781.38" xr:uid="{782B69DE-8E85-4D8F-9DAC-8EB607F3F04E}"/>
+    <hyperlink ref="E5" r:id="rId7" xr:uid="{9A588C41-B2AF-4BF7-9A00-6DD9FB5CABFD}"/>
+    <hyperlink ref="F5" r:id="rId8" display="https://osf.io/8k9nt/" xr:uid="{159ED34F-FF9E-488E-B419-5DB75A1053A4}"/>
+    <hyperlink ref="C6" r:id="rId9" display="https://doi.org/10.15626/MP.2022.3236" xr:uid="{365B7B56-6668-4E66-B95F-686BDD31EEE7}"/>
+    <hyperlink ref="E6" r:id="rId10" xr:uid="{6F806BFE-1E43-477A-98D8-853E317AB860}"/>
+    <hyperlink ref="G6" r:id="rId11" xr:uid="{39191331-4837-4425-955D-F7F137894FA7}"/>
+    <hyperlink ref="E7" r:id="rId12" xr:uid="{BF2F029F-64B8-458D-9E6D-FB7B0A9D9E54}"/>
+    <hyperlink ref="G7" r:id="rId13" xr:uid="{130EB372-4CDB-40F4-B733-C289D48B1C4C}"/>
+    <hyperlink ref="C8" r:id="rId14" display="https://doi.org/10.15626/MP.2020.2639" xr:uid="{B96128B1-8C8B-4E74-8D94-6ECC038C9AAC}"/>
+    <hyperlink ref="E8" r:id="rId15" xr:uid="{AD4669E7-2751-41A0-BCE5-14632257828B}"/>
+    <hyperlink ref="G8" r:id="rId16" xr:uid="{3D2FC1C8-D1F7-407E-B397-D60D8B7AA2EA}"/>
+    <hyperlink ref="C9" r:id="rId17" display="https://doi.org/10.5334/jopd.92" xr:uid="{A071F59A-946C-461F-A4B7-033C6C45173A}"/>
+    <hyperlink ref="C10" r:id="rId18" display="https://doi.org/10.1016/j.jbusres.2023.114189" xr:uid="{51055E7B-DEE6-4A19-92E4-D1721DF822B1}"/>
+    <hyperlink ref="E10" r:id="rId19" xr:uid="{ED578A9E-FF99-4C7B-8A91-7C05D3B75022}"/>
+    <hyperlink ref="G10" r:id="rId20" xr:uid="{9BB5D8E7-F006-4255-8265-71EA7D3EBCE4}"/>
+    <hyperlink ref="C11" r:id="rId21" display="http://doi.org/10.5334/jopd.67" xr:uid="{C4050047-C1E1-404E-B073-E0C05CE8D173}"/>
+    <hyperlink ref="E11" r:id="rId22" xr:uid="{E3FEC74A-0F6F-4FFC-8AC0-B45670656896}"/>
+    <hyperlink ref="G11" r:id="rId23" xr:uid="{5C54A4BE-8B8C-494A-B29D-49F490A2C1C2}"/>
+    <hyperlink ref="C12" r:id="rId24" display="https://doi.org/10.1073/pnas.212037711" xr:uid="{C93D8067-4FC0-4D8D-8E47-D00FBE2F6608}"/>
+    <hyperlink ref="C13" r:id="rId25" display="https://doi.org/10.1037/bul0000356" xr:uid="{BDFC91BF-1233-4C67-A06A-DDE12D0F8BEB}"/>
+    <hyperlink ref="E13" r:id="rId26" xr:uid="{D92AA8D7-14D0-4433-B7CB-0E1DF9F275E9}"/>
+    <hyperlink ref="F13" r:id="rId27" xr:uid="{FB02A3AD-7B15-4C0E-9F16-631065DCF554}"/>
+    <hyperlink ref="C14" r:id="rId28" display="https://doi.org/10.1080/02699931.2021.1979473" xr:uid="{AD06D523-F5DB-442E-B989-A6C32B777ED1}"/>
+    <hyperlink ref="E14" r:id="rId29" xr:uid="{7BB9E6E9-A4CD-49AA-A55E-7BDA3DFBBEC0}"/>
+    <hyperlink ref="F14" r:id="rId30" xr:uid="{21E90428-3D65-4277-B80F-141F81A55916}"/>
+    <hyperlink ref="C15" r:id="rId31" display="https://doi.org/10.1016/j.jesp.2020.104066" xr:uid="{2A8C850C-91E2-46B0-987D-55EB0D9C3B0F}"/>
+    <hyperlink ref="E15" r:id="rId32" display="https://osf.io/96de2" xr:uid="{6C52A618-C82D-476C-89C8-16F20F642485}"/>
+    <hyperlink ref="C16" r:id="rId33" display="https://doi.org/10.5964/ejop.2639" xr:uid="{0DFC4B36-9C4B-4E2A-92F6-E6D628E09B18}"/>
+    <hyperlink ref="C17" r:id="rId34" display="https://doi.org/10.1177/1745691620984474" xr:uid="{54D1B1A1-B51A-4CA8-9C8A-8B2BF483FDDC}"/>
+    <hyperlink ref="C18" r:id="rId35" display="https://doi.org/10.1016/j.jesp.2020.104060" xr:uid="{862E7504-584A-4242-9B75-22375BC49E27}"/>
+    <hyperlink ref="C19" r:id="rId36" display="https://doi.org/10.1016/j.jesp.2019.103942" xr:uid="{B8F41347-13BD-4D71-A682-6BD22F709DE9}"/>
+    <hyperlink ref="C20" r:id="rId37" display="https://doi.org/10.1037/bul0000220" xr:uid="{065B9BF3-E67C-451C-B12A-2782BA816965}"/>
+    <hyperlink ref="G20" r:id="rId38" display="https://www.researchgate.net/publication/337261659_Crowdsourcing_Hypothesis_Tests_Making_Transparent_How_Design_Choices_Shape_Research_Results" xr:uid="{099DB906-00A3-4756-8332-B3B87A0D9EEF}"/>
+    <hyperlink ref="C21" r:id="rId39" display="https://osf.io/34sv6" xr:uid="{DD65BC2F-BFCE-4797-B982-DFEB045FD826}"/>
+    <hyperlink ref="G21" r:id="rId40" xr:uid="{87350DFD-AAFD-4459-9249-138523C66895}"/>
+    <hyperlink ref="C22" r:id="rId41" display="https://doi.org/10.31234/osf.io/akfzh" xr:uid="{9B39A2DF-F148-4367-8E24-E1AFFA69762A}"/>
+    <hyperlink ref="F22" r:id="rId42" xr:uid="{BACE566D-5B6D-4E9A-81EF-685F01A92950}"/>
+    <hyperlink ref="C23" r:id="rId43" display="https://doi.org/10.31234/osf.io/gj76p" xr:uid="{B34F1845-E395-44F6-9C3F-A1DC39394D59}"/>
+    <hyperlink ref="C24" r:id="rId44" display="https://doi.org/10.31234/osf.io/krwcn" xr:uid="{BEF8554E-090A-4B5A-89F1-432B57FC20C6}"/>
+    <hyperlink ref="G24" r:id="rId45" xr:uid="{5C9D188F-41F0-4255-9A7F-776DC0D7C6B3}"/>
+    <hyperlink ref="C25" r:id="rId46" display="https://osf.io/preprints/metaarxiv/ewb2t" xr:uid="{73F38CDC-AE74-42AE-9875-B80E70CAAD04}"/>
+    <hyperlink ref="G25" r:id="rId47" xr:uid="{F242B96D-FDF5-4CE7-BDFB-CFE6A00240A0}"/>
+    <hyperlink ref="C26" r:id="rId48" display="https://osf.io/8cwpy" xr:uid="{092A1365-FCB4-41FB-8313-CF735B66A2DD}"/>
+    <hyperlink ref="E26" r:id="rId49" xr:uid="{ECBA28D3-FB1C-4193-901B-41108340BCFD}"/>
+    <hyperlink ref="F26" r:id="rId50" display="https://osf.io/c2ynz" xr:uid="{E93BA08A-3A49-4D35-AC66-D74574AF96C4}"/>
+    <hyperlink ref="C28" r:id="rId51" display="https://doi.org/10.31222/osf.io/8psw2" xr:uid="{C0F54102-918A-4578-B027-C78823FD4B7D}"/>
+    <hyperlink ref="F28" r:id="rId52" xr:uid="{97ACEB9A-0C43-4AA2-ACFE-F50A4B6B56F0}"/>
+    <hyperlink ref="C29" r:id="rId53" display="https://doi.org/10.31234/osf.io/2kfh3" xr:uid="{FE4142A2-4633-4F53-8F23-5F50CB46E97C}"/>
+    <hyperlink ref="F29" r:id="rId54" xr:uid="{174B565C-80A9-4205-A2B1-E2DC35E916D7}"/>
+    <hyperlink ref="C30" r:id="rId55" display="https://doi.org/10.31234/osf.io/ntukz" xr:uid="{562912E7-E3CF-4637-A5EC-F5598C18FAED}"/>
+    <hyperlink ref="F30" r:id="rId56" display="https://osf.io/7pw4c/" xr:uid="{E5872E1A-19BD-48E3-BBC5-0325DE4F50E7}"/>
+    <hyperlink ref="C31" r:id="rId57" display="https://doi.org/10.31234/osf.io/wf2tn" xr:uid="{A453771E-19D2-48CD-8D51-59EE29E521DB}"/>
+    <hyperlink ref="C32" r:id="rId58" display="https://doi.org/10.31219/osf.io/2tr6q" xr:uid="{0F998EE8-1C6C-4120-A8A7-D2F043592BCD}"/>
+    <hyperlink ref="F32" r:id="rId59" display="https://osf.io/9qz3d" xr:uid="{4BBBB1B2-2501-4EEF-8BB3-87C7A2170367}"/>
+    <hyperlink ref="C33" r:id="rId60" display="https://doi.org/10.31234/osf.io/hjbwp" xr:uid="{519680D7-CB35-4C47-AB82-99AC96EA8DFE}"/>
+    <hyperlink ref="C34" r:id="rId61" display="https://doi.org/10.31234/osf.io/mt49r" xr:uid="{9EA40F6E-B1C1-4A75-B481-39C90A03E75E}"/>
+    <hyperlink ref="C35" r:id="rId62" display="https://doi.org/10.31234/osf.io/bnsx2" xr:uid="{63D5CDF4-C3ED-4621-886B-026265E45F56}"/>
+    <hyperlink ref="E35" r:id="rId63" xr:uid="{08AABF7C-2FA2-46EF-98CF-56A84170523F}"/>
+    <hyperlink ref="C2" r:id="rId64" display="https://doi.org/10.1007/s41449-025-00460-x" xr:uid="{A0B3F658-F0ED-4C9D-BD5A-8C5E0B28DDAD}"/>
+    <hyperlink ref="E2" r:id="rId65" xr:uid="{86E48510-5694-4822-9C15-811C53298144}"/>
+    <hyperlink ref="F2" r:id="rId66" xr:uid="{F2CF54DC-82BB-4B77-9942-9BF93FA7F0A6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId64"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId67"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added stage 1 RR; corrected preprint vs. green OA distinction in research table
</commit_message>
<xml_diff>
--- a/research.xlsx
+++ b/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lroesele.IVV5NET\sciebo - Röseler, Lukas (lroesele@uni-muenster.de)@uni-muenster.sciebo.de\LeaRn\home\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DE5604-9A5C-4E42-A77C-7871E3730DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B5DDEC-62BD-4096-B0D5-082A84ADD0CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AAC91D46-EE41-4CEB-9A66-251368506452}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="144">
   <si>
     <t>#</t>
   </si>
@@ -125,9 +125,6 @@
     <t>https://doi.org/10.5281/zenodo.13945051</t>
   </si>
   <si>
-    <t>Green</t>
-  </si>
-  <si>
     <t>Replication / Anchoring</t>
   </si>
   <si>
@@ -588,6 +585,51 @@
   </si>
   <si>
     <t>https://doi.org/10.5281/zenodo.15487804</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Rebholz, T. R., Groß, J., &amp; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Röseler, L.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (2025, June 24). Assimilation to External Cues: Comparing the Reliability of Anchoring Effects, Advice Taking, and Hindsight Bias and Exploring its Determinants. https://doi.org/10.31234/osf.io/5u8br_v1</t>
+    </r>
+  </si>
+  <si>
+    <t>Preprint</t>
+  </si>
+  <si>
+    <t>https://osf.io/4n3am/</t>
+  </si>
+  <si>
+    <t>tbd</t>
+  </si>
+  <si>
+    <t>https://osf.io/preprints/psyarxiv/5u8br_v1</t>
   </si>
 </sst>
 </file>
@@ -1003,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D3A1534-13D7-4FF4-8CD6-0F369116C1B6}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,10 +1067,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -1037,334 +1079,340 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>15</v>
+        <v>140</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="F2" s="9"/>
+        <v>141</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>142</v>
+      </c>
       <c r="G2" s="11" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="9"/>
       <c r="F3" s="9"/>
       <c r="G3" s="11" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="1"/>
       <c r="H4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="7"/>
+      <c r="G5" s="1"/>
       <c r="H5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
+        <v>32</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>31</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>30</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="C8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="F8" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>29</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>123</v>
+        <v>21</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>30</v>
+        <v>25</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>122</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>35</v>
+        <v>19</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="4" t="s">
-        <v>40</v>
+        <v>33</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>29</v>
+        <v>37</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="4" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="7"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
+      <c r="G14" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="H14" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>48</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="2" t="s">
         <v>10</v>
@@ -1372,108 +1420,114 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="7"/>
+        <v>45</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="E16" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="7"/>
+        <v>48</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="E17" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>124</v>
+        <v>49</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+        <v>51</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>123</v>
+      </c>
       <c r="G18" s="7"/>
       <c r="H18" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>35</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="G20" s="7"/>
       <c r="H20" s="2" t="s">
@@ -1482,20 +1536,22 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" s="7"/>
+        <v>57</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="E21" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G21" s="7"/>
       <c r="H21" s="2" t="s">
@@ -1504,47 +1560,49 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" s="7"/>
+        <v>62</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="E22" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>69</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="G22" s="7"/>
       <c r="H22" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>20</v>
+        <v>65</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F23" s="7"/>
+        <v>66</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="G23" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>10</v>
@@ -1552,25 +1610,23 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
+      </c>
+      <c r="F24" s="7"/>
+      <c r="G24" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>10</v>
@@ -1578,23 +1634,25 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>15</v>
+        <v>140</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F25" s="7"/>
+        <v>74</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="G25" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>10</v>
@@ -1602,25 +1660,23 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>82</v>
-      </c>
       <c r="D26" s="2" t="s">
-        <v>15</v>
+        <v>140</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
+      </c>
+      <c r="F26" s="7"/>
+      <c r="G26" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>10</v>
@@ -1628,359 +1684,387 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="C27" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>10</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E27" s="2" t="s">
+      <c r="F28" s="7"/>
+      <c r="G28" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="4" t="s">
+      <c r="H28" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>9</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="H27" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>9</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" s="4" t="s">
+      <c r="D29" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" s="4" t="s">
+      <c r="F29" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G29" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F28" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>8.5</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="H29" s="2" t="s">
-        <v>94</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>15</v>
+        <v>140</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>97</v>
+        <v>91</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>21</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
+        <v>8</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
         <v>7</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="D31" s="2" t="s">
+      <c r="B32" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="G31" s="2" t="s">
+    </row>
+    <row r="33" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="D33" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>5</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="G34" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>4</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>3</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>6</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>5</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F33" s="7"/>
-      <c r="G33" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="150" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <v>4</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="F34" s="5" t="s">
+      <c r="C36" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F36" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="G34" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
-        <v>3</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E35" s="2" t="s">
+      <c r="G36" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F35" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
-        <v>2</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="H36" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
+        <v>2</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
         <v>1</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B38" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="D38" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37" s="4" t="s">
+      <c r="F38" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="G38" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="G37" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="H37" s="2" t="s">
+      <c r="H38" s="2" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E5" r:id="rId1" xr:uid="{41A1C6B5-F794-4E36-A76C-521B33FA2C7E}"/>
-    <hyperlink ref="F5" r:id="rId2" xr:uid="{D45BBE43-E931-4EDA-AB62-49ECCD4358D7}"/>
-    <hyperlink ref="C6" r:id="rId3" display="https://doi.org/10.5281/zenodo.13945051" xr:uid="{15B1DF19-42C9-4721-BDEE-790C2BD36401}"/>
-    <hyperlink ref="E6" r:id="rId4" xr:uid="{EE424F71-99CE-4EE2-B51B-A911BE1F8393}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{3F25FBC9-AB32-4C97-9E08-65B039840DB8}"/>
-    <hyperlink ref="C7" r:id="rId6" display="https://doi.org/10.18718/81781.38" xr:uid="{782B69DE-8E85-4D8F-9DAC-8EB607F3F04E}"/>
-    <hyperlink ref="E7" r:id="rId7" xr:uid="{9A588C41-B2AF-4BF7-9A00-6DD9FB5CABFD}"/>
-    <hyperlink ref="F7" r:id="rId8" display="https://osf.io/8k9nt/" xr:uid="{159ED34F-FF9E-488E-B419-5DB75A1053A4}"/>
-    <hyperlink ref="C8" r:id="rId9" display="https://doi.org/10.15626/MP.2022.3236" xr:uid="{365B7B56-6668-4E66-B95F-686BDD31EEE7}"/>
-    <hyperlink ref="E8" r:id="rId10" xr:uid="{6F806BFE-1E43-477A-98D8-853E317AB860}"/>
-    <hyperlink ref="G8" r:id="rId11" xr:uid="{39191331-4837-4425-955D-F7F137894FA7}"/>
-    <hyperlink ref="E9" r:id="rId12" xr:uid="{BF2F029F-64B8-458D-9E6D-FB7B0A9D9E54}"/>
-    <hyperlink ref="G9" r:id="rId13" xr:uid="{130EB372-4CDB-40F4-B733-C289D48B1C4C}"/>
-    <hyperlink ref="C10" r:id="rId14" display="https://doi.org/10.15626/MP.2020.2639" xr:uid="{B96128B1-8C8B-4E74-8D94-6ECC038C9AAC}"/>
-    <hyperlink ref="E10" r:id="rId15" xr:uid="{AD4669E7-2751-41A0-BCE5-14632257828B}"/>
-    <hyperlink ref="G10" r:id="rId16" xr:uid="{3D2FC1C8-D1F7-407E-B397-D60D8B7AA2EA}"/>
-    <hyperlink ref="C11" r:id="rId17" display="https://doi.org/10.5334/jopd.92" xr:uid="{A071F59A-946C-461F-A4B7-033C6C45173A}"/>
-    <hyperlink ref="C12" r:id="rId18" display="https://doi.org/10.1016/j.jbusres.2023.114189" xr:uid="{51055E7B-DEE6-4A19-92E4-D1721DF822B1}"/>
-    <hyperlink ref="E12" r:id="rId19" xr:uid="{ED578A9E-FF99-4C7B-8A91-7C05D3B75022}"/>
-    <hyperlink ref="G12" r:id="rId20" xr:uid="{9BB5D8E7-F006-4255-8265-71EA7D3EBCE4}"/>
-    <hyperlink ref="C13" r:id="rId21" display="http://doi.org/10.5334/jopd.67" xr:uid="{C4050047-C1E1-404E-B073-E0C05CE8D173}"/>
-    <hyperlink ref="E13" r:id="rId22" xr:uid="{E3FEC74A-0F6F-4FFC-8AC0-B45670656896}"/>
-    <hyperlink ref="G13" r:id="rId23" xr:uid="{5C54A4BE-8B8C-494A-B29D-49F490A2C1C2}"/>
-    <hyperlink ref="C14" r:id="rId24" display="https://doi.org/10.1073/pnas.212037711" xr:uid="{C93D8067-4FC0-4D8D-8E47-D00FBE2F6608}"/>
-    <hyperlink ref="C15" r:id="rId25" display="https://doi.org/10.1037/bul0000356" xr:uid="{BDFC91BF-1233-4C67-A06A-DDE12D0F8BEB}"/>
-    <hyperlink ref="E15" r:id="rId26" xr:uid="{D92AA8D7-14D0-4433-B7CB-0E1DF9F275E9}"/>
-    <hyperlink ref="F15" r:id="rId27" xr:uid="{FB02A3AD-7B15-4C0E-9F16-631065DCF554}"/>
-    <hyperlink ref="C16" r:id="rId28" display="https://doi.org/10.1080/02699931.2021.1979473" xr:uid="{AD06D523-F5DB-442E-B989-A6C32B777ED1}"/>
-    <hyperlink ref="E16" r:id="rId29" xr:uid="{7BB9E6E9-A4CD-49AA-A55E-7BDA3DFBBEC0}"/>
-    <hyperlink ref="F16" r:id="rId30" xr:uid="{21E90428-3D65-4277-B80F-141F81A55916}"/>
-    <hyperlink ref="C17" r:id="rId31" display="https://doi.org/10.1016/j.jesp.2020.104066" xr:uid="{2A8C850C-91E2-46B0-987D-55EB0D9C3B0F}"/>
-    <hyperlink ref="E17" r:id="rId32" display="https://osf.io/96de2" xr:uid="{6C52A618-C82D-476C-89C8-16F20F642485}"/>
-    <hyperlink ref="C18" r:id="rId33" display="https://doi.org/10.5964/ejop.2639" xr:uid="{0DFC4B36-9C4B-4E2A-92F6-E6D628E09B18}"/>
-    <hyperlink ref="C19" r:id="rId34" display="https://doi.org/10.1177/1745691620984474" xr:uid="{54D1B1A1-B51A-4CA8-9C8A-8B2BF483FDDC}"/>
-    <hyperlink ref="C20" r:id="rId35" display="https://doi.org/10.1016/j.jesp.2020.104060" xr:uid="{862E7504-584A-4242-9B75-22375BC49E27}"/>
-    <hyperlink ref="C21" r:id="rId36" display="https://doi.org/10.1016/j.jesp.2019.103942" xr:uid="{B8F41347-13BD-4D71-A682-6BD22F709DE9}"/>
-    <hyperlink ref="C22" r:id="rId37" display="https://doi.org/10.1037/bul0000220" xr:uid="{065B9BF3-E67C-451C-B12A-2782BA816965}"/>
-    <hyperlink ref="G22" r:id="rId38" display="https://www.researchgate.net/publication/337261659_Crowdsourcing_Hypothesis_Tests_Making_Transparent_How_Design_Choices_Shape_Research_Results" xr:uid="{099DB906-00A3-4756-8332-B3B87A0D9EEF}"/>
-    <hyperlink ref="C23" r:id="rId39" display="https://osf.io/34sv6" xr:uid="{DD65BC2F-BFCE-4797-B982-DFEB045FD826}"/>
-    <hyperlink ref="G23" r:id="rId40" xr:uid="{87350DFD-AAFD-4459-9249-138523C66895}"/>
-    <hyperlink ref="C24" r:id="rId41" display="https://doi.org/10.31234/osf.io/akfzh" xr:uid="{9B39A2DF-F148-4367-8E24-E1AFFA69762A}"/>
-    <hyperlink ref="F24" r:id="rId42" xr:uid="{BACE566D-5B6D-4E9A-81EF-685F01A92950}"/>
-    <hyperlink ref="C25" r:id="rId43" display="https://doi.org/10.31234/osf.io/gj76p" xr:uid="{B34F1845-E395-44F6-9C3F-A1DC39394D59}"/>
-    <hyperlink ref="C26" r:id="rId44" display="https://doi.org/10.31234/osf.io/krwcn" xr:uid="{BEF8554E-090A-4B5A-89F1-432B57FC20C6}"/>
-    <hyperlink ref="G26" r:id="rId45" xr:uid="{5C9D188F-41F0-4255-9A7F-776DC0D7C6B3}"/>
-    <hyperlink ref="C27" r:id="rId46" display="https://osf.io/preprints/metaarxiv/ewb2t" xr:uid="{73F38CDC-AE74-42AE-9875-B80E70CAAD04}"/>
-    <hyperlink ref="G27" r:id="rId47" xr:uid="{F242B96D-FDF5-4CE7-BDFB-CFE6A00240A0}"/>
-    <hyperlink ref="C28" r:id="rId48" display="https://osf.io/8cwpy" xr:uid="{092A1365-FCB4-41FB-8313-CF735B66A2DD}"/>
-    <hyperlink ref="E28" r:id="rId49" xr:uid="{ECBA28D3-FB1C-4193-901B-41108340BCFD}"/>
-    <hyperlink ref="F28" r:id="rId50" display="https://osf.io/c2ynz" xr:uid="{E93BA08A-3A49-4D35-AC66-D74574AF96C4}"/>
-    <hyperlink ref="C30" r:id="rId51" display="https://doi.org/10.31222/osf.io/8psw2" xr:uid="{C0F54102-918A-4578-B027-C78823FD4B7D}"/>
-    <hyperlink ref="F30" r:id="rId52" xr:uid="{97ACEB9A-0C43-4AA2-ACFE-F50A4B6B56F0}"/>
-    <hyperlink ref="C31" r:id="rId53" display="https://doi.org/10.31234/osf.io/2kfh3" xr:uid="{FE4142A2-4633-4F53-8F23-5F50CB46E97C}"/>
-    <hyperlink ref="F31" r:id="rId54" xr:uid="{174B565C-80A9-4205-A2B1-E2DC35E916D7}"/>
-    <hyperlink ref="C32" r:id="rId55" display="https://doi.org/10.31234/osf.io/ntukz" xr:uid="{562912E7-E3CF-4637-A5EC-F5598C18FAED}"/>
-    <hyperlink ref="F32" r:id="rId56" display="https://osf.io/7pw4c/" xr:uid="{E5872E1A-19BD-48E3-BBC5-0325DE4F50E7}"/>
-    <hyperlink ref="C33" r:id="rId57" display="https://doi.org/10.31234/osf.io/wf2tn" xr:uid="{A453771E-19D2-48CD-8D51-59EE29E521DB}"/>
-    <hyperlink ref="C34" r:id="rId58" display="https://doi.org/10.31219/osf.io/2tr6q" xr:uid="{0F998EE8-1C6C-4120-A8A7-D2F043592BCD}"/>
-    <hyperlink ref="F34" r:id="rId59" display="https://osf.io/9qz3d" xr:uid="{4BBBB1B2-2501-4EEF-8BB3-87C7A2170367}"/>
-    <hyperlink ref="C35" r:id="rId60" display="https://doi.org/10.31234/osf.io/hjbwp" xr:uid="{519680D7-CB35-4C47-AB82-99AC96EA8DFE}"/>
-    <hyperlink ref="C36" r:id="rId61" display="https://doi.org/10.31234/osf.io/mt49r" xr:uid="{9EA40F6E-B1C1-4A75-B481-39C90A03E75E}"/>
-    <hyperlink ref="C37" r:id="rId62" display="https://doi.org/10.31234/osf.io/bnsx2" xr:uid="{63D5CDF4-C3ED-4621-886B-026265E45F56}"/>
-    <hyperlink ref="E37" r:id="rId63" xr:uid="{08AABF7C-2FA2-46EF-98CF-56A84170523F}"/>
-    <hyperlink ref="C4" r:id="rId64" display="https://doi.org/10.1007/s41449-025-00460-x" xr:uid="{A0B3F658-F0ED-4C9D-BD5A-8C5E0B28DDAD}"/>
-    <hyperlink ref="E4" r:id="rId65" xr:uid="{86E48510-5694-4822-9C15-811C53298144}"/>
-    <hyperlink ref="F4" r:id="rId66" xr:uid="{F2CF54DC-82BB-4B77-9942-9BF93FA7F0A6}"/>
-    <hyperlink ref="G3" r:id="rId67" xr:uid="{C48C75DC-DB55-4450-A4F7-E9E0C34ECC15}"/>
-    <hyperlink ref="E2" r:id="rId68" xr:uid="{18606C55-07D2-45E4-8557-E96814F20E71}"/>
-    <hyperlink ref="G2" r:id="rId69" xr:uid="{080935E3-AB10-41DA-A9E4-594385CA18FB}"/>
+    <hyperlink ref="E6" r:id="rId1" xr:uid="{41A1C6B5-F794-4E36-A76C-521B33FA2C7E}"/>
+    <hyperlink ref="F6" r:id="rId2" xr:uid="{D45BBE43-E931-4EDA-AB62-49ECCD4358D7}"/>
+    <hyperlink ref="C7" r:id="rId3" display="https://doi.org/10.5281/zenodo.13945051" xr:uid="{15B1DF19-42C9-4721-BDEE-790C2BD36401}"/>
+    <hyperlink ref="E7" r:id="rId4" xr:uid="{EE424F71-99CE-4EE2-B51B-A911BE1F8393}"/>
+    <hyperlink ref="G7" r:id="rId5" xr:uid="{3F25FBC9-AB32-4C97-9E08-65B039840DB8}"/>
+    <hyperlink ref="C8" r:id="rId6" display="https://doi.org/10.18718/81781.38" xr:uid="{782B69DE-8E85-4D8F-9DAC-8EB607F3F04E}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{9A588C41-B2AF-4BF7-9A00-6DD9FB5CABFD}"/>
+    <hyperlink ref="F8" r:id="rId8" display="https://osf.io/8k9nt/" xr:uid="{159ED34F-FF9E-488E-B419-5DB75A1053A4}"/>
+    <hyperlink ref="C9" r:id="rId9" display="https://doi.org/10.15626/MP.2022.3236" xr:uid="{365B7B56-6668-4E66-B95F-686BDD31EEE7}"/>
+    <hyperlink ref="E9" r:id="rId10" xr:uid="{6F806BFE-1E43-477A-98D8-853E317AB860}"/>
+    <hyperlink ref="G9" r:id="rId11" xr:uid="{39191331-4837-4425-955D-F7F137894FA7}"/>
+    <hyperlink ref="E10" r:id="rId12" xr:uid="{BF2F029F-64B8-458D-9E6D-FB7B0A9D9E54}"/>
+    <hyperlink ref="G10" r:id="rId13" xr:uid="{130EB372-4CDB-40F4-B733-C289D48B1C4C}"/>
+    <hyperlink ref="C11" r:id="rId14" display="https://doi.org/10.15626/MP.2020.2639" xr:uid="{B96128B1-8C8B-4E74-8D94-6ECC038C9AAC}"/>
+    <hyperlink ref="E11" r:id="rId15" xr:uid="{AD4669E7-2751-41A0-BCE5-14632257828B}"/>
+    <hyperlink ref="G11" r:id="rId16" xr:uid="{3D2FC1C8-D1F7-407E-B397-D60D8B7AA2EA}"/>
+    <hyperlink ref="C12" r:id="rId17" display="https://doi.org/10.5334/jopd.92" xr:uid="{A071F59A-946C-461F-A4B7-033C6C45173A}"/>
+    <hyperlink ref="C13" r:id="rId18" display="https://doi.org/10.1016/j.jbusres.2023.114189" xr:uid="{51055E7B-DEE6-4A19-92E4-D1721DF822B1}"/>
+    <hyperlink ref="E13" r:id="rId19" xr:uid="{ED578A9E-FF99-4C7B-8A91-7C05D3B75022}"/>
+    <hyperlink ref="G13" r:id="rId20" xr:uid="{9BB5D8E7-F006-4255-8265-71EA7D3EBCE4}"/>
+    <hyperlink ref="C14" r:id="rId21" display="http://doi.org/10.5334/jopd.67" xr:uid="{C4050047-C1E1-404E-B073-E0C05CE8D173}"/>
+    <hyperlink ref="E14" r:id="rId22" xr:uid="{E3FEC74A-0F6F-4FFC-8AC0-B45670656896}"/>
+    <hyperlink ref="G14" r:id="rId23" xr:uid="{5C54A4BE-8B8C-494A-B29D-49F490A2C1C2}"/>
+    <hyperlink ref="C15" r:id="rId24" display="https://doi.org/10.1073/pnas.212037711" xr:uid="{C93D8067-4FC0-4D8D-8E47-D00FBE2F6608}"/>
+    <hyperlink ref="C16" r:id="rId25" display="https://doi.org/10.1037/bul0000356" xr:uid="{BDFC91BF-1233-4C67-A06A-DDE12D0F8BEB}"/>
+    <hyperlink ref="E16" r:id="rId26" xr:uid="{D92AA8D7-14D0-4433-B7CB-0E1DF9F275E9}"/>
+    <hyperlink ref="F16" r:id="rId27" xr:uid="{FB02A3AD-7B15-4C0E-9F16-631065DCF554}"/>
+    <hyperlink ref="C17" r:id="rId28" display="https://doi.org/10.1080/02699931.2021.1979473" xr:uid="{AD06D523-F5DB-442E-B989-A6C32B777ED1}"/>
+    <hyperlink ref="E17" r:id="rId29" xr:uid="{7BB9E6E9-A4CD-49AA-A55E-7BDA3DFBBEC0}"/>
+    <hyperlink ref="F17" r:id="rId30" xr:uid="{21E90428-3D65-4277-B80F-141F81A55916}"/>
+    <hyperlink ref="C18" r:id="rId31" display="https://doi.org/10.1016/j.jesp.2020.104066" xr:uid="{2A8C850C-91E2-46B0-987D-55EB0D9C3B0F}"/>
+    <hyperlink ref="E18" r:id="rId32" display="https://osf.io/96de2" xr:uid="{6C52A618-C82D-476C-89C8-16F20F642485}"/>
+    <hyperlink ref="C19" r:id="rId33" display="https://doi.org/10.5964/ejop.2639" xr:uid="{0DFC4B36-9C4B-4E2A-92F6-E6D628E09B18}"/>
+    <hyperlink ref="C20" r:id="rId34" display="https://doi.org/10.1177/1745691620984474" xr:uid="{54D1B1A1-B51A-4CA8-9C8A-8B2BF483FDDC}"/>
+    <hyperlink ref="C21" r:id="rId35" display="https://doi.org/10.1016/j.jesp.2020.104060" xr:uid="{862E7504-584A-4242-9B75-22375BC49E27}"/>
+    <hyperlink ref="C22" r:id="rId36" display="https://doi.org/10.1016/j.jesp.2019.103942" xr:uid="{B8F41347-13BD-4D71-A682-6BD22F709DE9}"/>
+    <hyperlink ref="C23" r:id="rId37" display="https://doi.org/10.1037/bul0000220" xr:uid="{065B9BF3-E67C-451C-B12A-2782BA816965}"/>
+    <hyperlink ref="G23" r:id="rId38" display="https://www.researchgate.net/publication/337261659_Crowdsourcing_Hypothesis_Tests_Making_Transparent_How_Design_Choices_Shape_Research_Results" xr:uid="{099DB906-00A3-4756-8332-B3B87A0D9EEF}"/>
+    <hyperlink ref="C24" r:id="rId39" display="https://osf.io/34sv6" xr:uid="{DD65BC2F-BFCE-4797-B982-DFEB045FD826}"/>
+    <hyperlink ref="G24" r:id="rId40" xr:uid="{87350DFD-AAFD-4459-9249-138523C66895}"/>
+    <hyperlink ref="C25" r:id="rId41" display="https://doi.org/10.31234/osf.io/akfzh" xr:uid="{9B39A2DF-F148-4367-8E24-E1AFFA69762A}"/>
+    <hyperlink ref="F25" r:id="rId42" xr:uid="{BACE566D-5B6D-4E9A-81EF-685F01A92950}"/>
+    <hyperlink ref="C26" r:id="rId43" display="https://doi.org/10.31234/osf.io/gj76p" xr:uid="{B34F1845-E395-44F6-9C3F-A1DC39394D59}"/>
+    <hyperlink ref="C27" r:id="rId44" display="https://doi.org/10.31234/osf.io/krwcn" xr:uid="{BEF8554E-090A-4B5A-89F1-432B57FC20C6}"/>
+    <hyperlink ref="G27" r:id="rId45" xr:uid="{5C9D188F-41F0-4255-9A7F-776DC0D7C6B3}"/>
+    <hyperlink ref="C28" r:id="rId46" display="https://osf.io/preprints/metaarxiv/ewb2t" xr:uid="{73F38CDC-AE74-42AE-9875-B80E70CAAD04}"/>
+    <hyperlink ref="G28" r:id="rId47" xr:uid="{F242B96D-FDF5-4CE7-BDFB-CFE6A00240A0}"/>
+    <hyperlink ref="C29" r:id="rId48" display="https://osf.io/8cwpy" xr:uid="{092A1365-FCB4-41FB-8313-CF735B66A2DD}"/>
+    <hyperlink ref="E29" r:id="rId49" xr:uid="{ECBA28D3-FB1C-4193-901B-41108340BCFD}"/>
+    <hyperlink ref="F29" r:id="rId50" display="https://osf.io/c2ynz" xr:uid="{E93BA08A-3A49-4D35-AC66-D74574AF96C4}"/>
+    <hyperlink ref="F31" r:id="rId51" xr:uid="{97ACEB9A-0C43-4AA2-ACFE-F50A4B6B56F0}"/>
+    <hyperlink ref="C32" r:id="rId52" display="https://doi.org/10.31234/osf.io/2kfh3" xr:uid="{FE4142A2-4633-4F53-8F23-5F50CB46E97C}"/>
+    <hyperlink ref="F32" r:id="rId53" xr:uid="{174B565C-80A9-4205-A2B1-E2DC35E916D7}"/>
+    <hyperlink ref="C33" r:id="rId54" display="https://doi.org/10.31234/osf.io/ntukz" xr:uid="{562912E7-E3CF-4637-A5EC-F5598C18FAED}"/>
+    <hyperlink ref="F33" r:id="rId55" display="https://osf.io/7pw4c/" xr:uid="{E5872E1A-19BD-48E3-BBC5-0325DE4F50E7}"/>
+    <hyperlink ref="C34" r:id="rId56" display="https://doi.org/10.31234/osf.io/wf2tn" xr:uid="{A453771E-19D2-48CD-8D51-59EE29E521DB}"/>
+    <hyperlink ref="C35" r:id="rId57" display="https://doi.org/10.31219/osf.io/2tr6q" xr:uid="{0F998EE8-1C6C-4120-A8A7-D2F043592BCD}"/>
+    <hyperlink ref="F35" r:id="rId58" display="https://osf.io/9qz3d" xr:uid="{4BBBB1B2-2501-4EEF-8BB3-87C7A2170367}"/>
+    <hyperlink ref="C36" r:id="rId59" display="https://doi.org/10.31234/osf.io/hjbwp" xr:uid="{519680D7-CB35-4C47-AB82-99AC96EA8DFE}"/>
+    <hyperlink ref="C37" r:id="rId60" display="https://doi.org/10.31234/osf.io/mt49r" xr:uid="{9EA40F6E-B1C1-4A75-B481-39C90A03E75E}"/>
+    <hyperlink ref="C38" r:id="rId61" display="https://doi.org/10.31234/osf.io/bnsx2" xr:uid="{63D5CDF4-C3ED-4621-886B-026265E45F56}"/>
+    <hyperlink ref="E38" r:id="rId62" xr:uid="{08AABF7C-2FA2-46EF-98CF-56A84170523F}"/>
+    <hyperlink ref="C5" r:id="rId63" display="https://doi.org/10.1007/s41449-025-00460-x" xr:uid="{A0B3F658-F0ED-4C9D-BD5A-8C5E0B28DDAD}"/>
+    <hyperlink ref="E5" r:id="rId64" xr:uid="{86E48510-5694-4822-9C15-811C53298144}"/>
+    <hyperlink ref="F5" r:id="rId65" xr:uid="{F2CF54DC-82BB-4B77-9942-9BF93FA7F0A6}"/>
+    <hyperlink ref="G4" r:id="rId66" xr:uid="{C48C75DC-DB55-4450-A4F7-E9E0C34ECC15}"/>
+    <hyperlink ref="E3" r:id="rId67" xr:uid="{18606C55-07D2-45E4-8557-E96814F20E71}"/>
+    <hyperlink ref="G3" r:id="rId68" xr:uid="{080935E3-AB10-41DA-A9E4-594385CA18FB}"/>
+    <hyperlink ref="E2" r:id="rId69" xr:uid="{CD47EA21-01E5-4F81-861D-1BCF591E3D8D}"/>
+    <hyperlink ref="G2" r:id="rId70" xr:uid="{DB58B12E-C04C-4B6A-99CE-11EF593D3E0F}"/>
+    <hyperlink ref="C31" r:id="rId71" display="https://doi.org/10.31222/osf.io/8psw2" xr:uid="{C0F54102-918A-4578-B027-C78823FD4B7D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId70"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId72"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated research and index, new render
</commit_message>
<xml_diff>
--- a/research.xlsx
+++ b/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lroesele.IVV5NET\sciebo - Röseler, Lukas (lroesele@uni-muenster.de)@uni-muenster.sciebo.de\LeaRn\home\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905D32AD-9FB6-4AB6-98CB-AB29809558EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C773C9B6-7E09-4C9A-A504-0B76C34582DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AAC91D46-EE41-4CEB-9A66-251368506452}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="151">
   <si>
     <t>#</t>
   </si>
@@ -722,6 +722,38 @@
       </rPr>
       <t>, Wallrich, L., Adler, S., Back, M., Busch, N., Dienlin, T., Evans, T. R., Goltermann, J., Hartmann, H., Horstmann, J., Korbmacher, M., Oppong Boakye, P., Richter, H., Richter, M., Silverstein, P., Steltenpohl, C. N., Syed, M., Vaidis, D., Verheyen, S., … Azevedo, F. (2025). Replication Research: Journal Description (R2 Launch). Zenodo. https://doi.org/10.5281/zenodo.17241396</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Röseler, L.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (2025, November 24). Preregistrations without Code do not Prevent P-Hacking. MetaArxiv. https://doi.org/10.31222/osf.io/v259t_v1  </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.31222/osf.io/v259t_v1  </t>
+  </si>
+  <si>
+    <t>https://doi.org/10.5281/zenodo.17241396</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.5281/zenodo.17279413</t>
   </si>
 </sst>
 </file>
@@ -811,7 +843,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -844,6 +876,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1159,10 +1197,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D3A1534-13D7-4FF4-8CD6-0F369116C1B6}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D2:D3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1198,253 +1236,255 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>146</v>
+        <v>41</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>147</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>140</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>148</v>
+      </c>
       <c r="H2" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>145</v>
+      <c r="C3" s="15" t="s">
+        <v>146</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>140</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="G3" s="9" t="s">
+        <v>149</v>
+      </c>
       <c r="H3" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>37</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>36</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="H5" s="2" t="s">
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>140</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="F6" s="9"/>
+        <v>141</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>142</v>
+      </c>
       <c r="G6" s="11" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="E7" s="9"/>
+      <c r="E7" s="9" t="s">
+        <v>137</v>
+      </c>
       <c r="F7" s="9"/>
       <c r="G7" s="11" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="1"/>
+        <v>140</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="11" t="s">
+        <v>134</v>
+      </c>
       <c r="H8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="7"/>
+      <c r="G9" s="1"/>
       <c r="H9" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
+        <v>32</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>31</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="4" t="s">
+      <c r="F11" s="7"/>
+      <c r="G11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="H11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>30</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>29</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>20</v>
@@ -1452,23 +1492,23 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>122</v>
+        <v>21</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>20</v>
@@ -1476,23 +1516,23 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>122</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>20</v>
@@ -1500,25 +1540,23 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>34</v>
+        <v>19</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="G15" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>20</v>
@@ -1526,91 +1564,93 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>28</v>
+        <v>37</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="4" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
+        <v>24</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="7"/>
       <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
+      <c r="G18" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="H18" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>47</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="2" t="s">
         <v>10</v>
@@ -1618,67 +1658,71 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G20" s="7"/>
       <c r="H20" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>123</v>
+        <v>49</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="G21" s="7"/>
       <c r="H21" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>19</v>
-      </c>
       <c r="B22" s="2" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+        <v>51</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>123</v>
+      </c>
       <c r="G22" s="7"/>
       <c r="H22" s="2" t="s">
         <v>20</v>
@@ -1686,46 +1730,42 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="G24" s="7"/>
       <c r="H24" s="2" t="s">
@@ -1734,22 +1774,22 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>9</v>
+        <v>57</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G25" s="7"/>
       <c r="H25" s="2" t="s">
@@ -1758,49 +1798,49 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>68</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="G26" s="7"/>
       <c r="H26" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>19</v>
+        <v>65</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F27" s="7"/>
+        <v>66</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="G27" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>10</v>
@@ -1808,25 +1848,23 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>140</v>
+        <v>19</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>10</v>
@@ -1834,23 +1872,25 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>140</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F29" s="7"/>
+        <v>74</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="G29" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>10</v>
@@ -1858,25 +1898,23 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>77</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>140</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
+      </c>
+      <c r="F30" s="7"/>
+      <c r="G30" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>10</v>
@@ -1884,361 +1922,389 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>140</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F31" s="7"/>
+        <v>34</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="G31" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E32" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>88</v>
+      <c r="E32" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F32" s="7"/>
+      <c r="G32" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>90</v>
+        <v>21</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>34</v>
+      <c r="E33" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>124</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>93</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>140</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>96</v>
+        <v>91</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>20</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>131</v>
+        <v>94</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>19</v>
+        <v>140</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
+        <v>7</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
         <v>6</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C37" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
-        <v>5</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>140</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F37" s="7"/>
+        <v>102</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>125</v>
+      </c>
       <c r="G37" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>140</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>126</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="F38" s="7"/>
       <c r="G38" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>140</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>127</v>
+        <v>108</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>140</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>34</v>
+        <v>111</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>127</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>116</v>
+        <v>41</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>1</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F42" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="G42" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="H42" s="2" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E9" r:id="rId1" xr:uid="{41A1C6B5-F794-4E36-A76C-521B33FA2C7E}"/>
-    <hyperlink ref="F9" r:id="rId2" xr:uid="{D45BBE43-E931-4EDA-AB62-49ECCD4358D7}"/>
-    <hyperlink ref="C10" r:id="rId3" display="https://doi.org/10.5281/zenodo.13945051" xr:uid="{15B1DF19-42C9-4721-BDEE-790C2BD36401}"/>
-    <hyperlink ref="E10" r:id="rId4" xr:uid="{EE424F71-99CE-4EE2-B51B-A911BE1F8393}"/>
-    <hyperlink ref="G10" r:id="rId5" xr:uid="{3F25FBC9-AB32-4C97-9E08-65B039840DB8}"/>
-    <hyperlink ref="C11" r:id="rId6" display="https://doi.org/10.18718/81781.38" xr:uid="{782B69DE-8E85-4D8F-9DAC-8EB607F3F04E}"/>
-    <hyperlink ref="E11" r:id="rId7" xr:uid="{9A588C41-B2AF-4BF7-9A00-6DD9FB5CABFD}"/>
-    <hyperlink ref="F11" r:id="rId8" display="https://osf.io/8k9nt/" xr:uid="{159ED34F-FF9E-488E-B419-5DB75A1053A4}"/>
-    <hyperlink ref="C12" r:id="rId9" display="https://doi.org/10.15626/MP.2022.3236" xr:uid="{365B7B56-6668-4E66-B95F-686BDD31EEE7}"/>
-    <hyperlink ref="E12" r:id="rId10" xr:uid="{6F806BFE-1E43-477A-98D8-853E317AB860}"/>
-    <hyperlink ref="G12" r:id="rId11" xr:uid="{39191331-4837-4425-955D-F7F137894FA7}"/>
-    <hyperlink ref="E13" r:id="rId12" xr:uid="{BF2F029F-64B8-458D-9E6D-FB7B0A9D9E54}"/>
-    <hyperlink ref="G13" r:id="rId13" xr:uid="{130EB372-4CDB-40F4-B733-C289D48B1C4C}"/>
-    <hyperlink ref="C14" r:id="rId14" display="https://doi.org/10.15626/MP.2020.2639" xr:uid="{B96128B1-8C8B-4E74-8D94-6ECC038C9AAC}"/>
-    <hyperlink ref="E14" r:id="rId15" xr:uid="{AD4669E7-2751-41A0-BCE5-14632257828B}"/>
-    <hyperlink ref="G14" r:id="rId16" xr:uid="{3D2FC1C8-D1F7-407E-B397-D60D8B7AA2EA}"/>
-    <hyperlink ref="C15" r:id="rId17" display="https://doi.org/10.5334/jopd.92" xr:uid="{A071F59A-946C-461F-A4B7-033C6C45173A}"/>
-    <hyperlink ref="C16" r:id="rId18" display="https://doi.org/10.1016/j.jbusres.2023.114189" xr:uid="{51055E7B-DEE6-4A19-92E4-D1721DF822B1}"/>
-    <hyperlink ref="E16" r:id="rId19" xr:uid="{ED578A9E-FF99-4C7B-8A91-7C05D3B75022}"/>
-    <hyperlink ref="G16" r:id="rId20" xr:uid="{9BB5D8E7-F006-4255-8265-71EA7D3EBCE4}"/>
-    <hyperlink ref="C17" r:id="rId21" display="http://doi.org/10.5334/jopd.67" xr:uid="{C4050047-C1E1-404E-B073-E0C05CE8D173}"/>
-    <hyperlink ref="E17" r:id="rId22" xr:uid="{E3FEC74A-0F6F-4FFC-8AC0-B45670656896}"/>
-    <hyperlink ref="G17" r:id="rId23" xr:uid="{5C54A4BE-8B8C-494A-B29D-49F490A2C1C2}"/>
-    <hyperlink ref="C18" r:id="rId24" display="https://doi.org/10.1073/pnas.212037711" xr:uid="{C93D8067-4FC0-4D8D-8E47-D00FBE2F6608}"/>
-    <hyperlink ref="C19" r:id="rId25" display="https://doi.org/10.1037/bul0000356" xr:uid="{BDFC91BF-1233-4C67-A06A-DDE12D0F8BEB}"/>
-    <hyperlink ref="E19" r:id="rId26" xr:uid="{D92AA8D7-14D0-4433-B7CB-0E1DF9F275E9}"/>
-    <hyperlink ref="F19" r:id="rId27" xr:uid="{FB02A3AD-7B15-4C0E-9F16-631065DCF554}"/>
-    <hyperlink ref="C20" r:id="rId28" display="https://doi.org/10.1080/02699931.2021.1979473" xr:uid="{AD06D523-F5DB-442E-B989-A6C32B777ED1}"/>
-    <hyperlink ref="E20" r:id="rId29" xr:uid="{7BB9E6E9-A4CD-49AA-A55E-7BDA3DFBBEC0}"/>
-    <hyperlink ref="F20" r:id="rId30" xr:uid="{21E90428-3D65-4277-B80F-141F81A55916}"/>
-    <hyperlink ref="C21" r:id="rId31" display="https://doi.org/10.1016/j.jesp.2020.104066" xr:uid="{2A8C850C-91E2-46B0-987D-55EB0D9C3B0F}"/>
-    <hyperlink ref="E21" r:id="rId32" display="https://osf.io/96de2" xr:uid="{6C52A618-C82D-476C-89C8-16F20F642485}"/>
-    <hyperlink ref="C22" r:id="rId33" display="https://doi.org/10.5964/ejop.2639" xr:uid="{0DFC4B36-9C4B-4E2A-92F6-E6D628E09B18}"/>
-    <hyperlink ref="C23" r:id="rId34" display="https://doi.org/10.1177/1745691620984474" xr:uid="{54D1B1A1-B51A-4CA8-9C8A-8B2BF483FDDC}"/>
-    <hyperlink ref="C24" r:id="rId35" display="https://doi.org/10.1016/j.jesp.2020.104060" xr:uid="{862E7504-584A-4242-9B75-22375BC49E27}"/>
-    <hyperlink ref="C25" r:id="rId36" display="https://doi.org/10.1016/j.jesp.2019.103942" xr:uid="{B8F41347-13BD-4D71-A682-6BD22F709DE9}"/>
-    <hyperlink ref="C26" r:id="rId37" display="https://doi.org/10.1037/bul0000220" xr:uid="{065B9BF3-E67C-451C-B12A-2782BA816965}"/>
-    <hyperlink ref="G26" r:id="rId38" display="https://www.researchgate.net/publication/337261659_Crowdsourcing_Hypothesis_Tests_Making_Transparent_How_Design_Choices_Shape_Research_Results" xr:uid="{099DB906-00A3-4756-8332-B3B87A0D9EEF}"/>
-    <hyperlink ref="C27" r:id="rId39" display="https://osf.io/34sv6" xr:uid="{DD65BC2F-BFCE-4797-B982-DFEB045FD826}"/>
-    <hyperlink ref="G27" r:id="rId40" xr:uid="{87350DFD-AAFD-4459-9249-138523C66895}"/>
-    <hyperlink ref="C28" r:id="rId41" display="https://doi.org/10.31234/osf.io/akfzh" xr:uid="{9B39A2DF-F148-4367-8E24-E1AFFA69762A}"/>
-    <hyperlink ref="F28" r:id="rId42" xr:uid="{BACE566D-5B6D-4E9A-81EF-685F01A92950}"/>
-    <hyperlink ref="C29" r:id="rId43" display="https://doi.org/10.31234/osf.io/gj76p" xr:uid="{B34F1845-E395-44F6-9C3F-A1DC39394D59}"/>
-    <hyperlink ref="C30" r:id="rId44" display="https://doi.org/10.31234/osf.io/krwcn" xr:uid="{BEF8554E-090A-4B5A-89F1-432B57FC20C6}"/>
-    <hyperlink ref="G30" r:id="rId45" xr:uid="{5C9D188F-41F0-4255-9A7F-776DC0D7C6B3}"/>
-    <hyperlink ref="C31" r:id="rId46" display="https://osf.io/preprints/metaarxiv/ewb2t" xr:uid="{73F38CDC-AE74-42AE-9875-B80E70CAAD04}"/>
-    <hyperlink ref="G31" r:id="rId47" xr:uid="{F242B96D-FDF5-4CE7-BDFB-CFE6A00240A0}"/>
-    <hyperlink ref="C32" r:id="rId48" display="https://osf.io/8cwpy" xr:uid="{092A1365-FCB4-41FB-8313-CF735B66A2DD}"/>
-    <hyperlink ref="E32" r:id="rId49" xr:uid="{ECBA28D3-FB1C-4193-901B-41108340BCFD}"/>
-    <hyperlink ref="F32" r:id="rId50" display="https://osf.io/c2ynz" xr:uid="{E93BA08A-3A49-4D35-AC66-D74574AF96C4}"/>
-    <hyperlink ref="F34" r:id="rId51" xr:uid="{97ACEB9A-0C43-4AA2-ACFE-F50A4B6B56F0}"/>
-    <hyperlink ref="C35" r:id="rId52" display="https://doi.org/10.31234/osf.io/2kfh3" xr:uid="{FE4142A2-4633-4F53-8F23-5F50CB46E97C}"/>
-    <hyperlink ref="F35" r:id="rId53" xr:uid="{174B565C-80A9-4205-A2B1-E2DC35E916D7}"/>
-    <hyperlink ref="C36" r:id="rId54" display="https://doi.org/10.31234/osf.io/ntukz" xr:uid="{562912E7-E3CF-4637-A5EC-F5598C18FAED}"/>
-    <hyperlink ref="F36" r:id="rId55" display="https://osf.io/7pw4c/" xr:uid="{E5872E1A-19BD-48E3-BBC5-0325DE4F50E7}"/>
-    <hyperlink ref="C37" r:id="rId56" display="https://doi.org/10.31234/osf.io/wf2tn" xr:uid="{A453771E-19D2-48CD-8D51-59EE29E521DB}"/>
-    <hyperlink ref="C38" r:id="rId57" display="https://doi.org/10.31219/osf.io/2tr6q" xr:uid="{0F998EE8-1C6C-4120-A8A7-D2F043592BCD}"/>
-    <hyperlink ref="F38" r:id="rId58" display="https://osf.io/9qz3d" xr:uid="{4BBBB1B2-2501-4EEF-8BB3-87C7A2170367}"/>
-    <hyperlink ref="C39" r:id="rId59" display="https://doi.org/10.31234/osf.io/hjbwp" xr:uid="{519680D7-CB35-4C47-AB82-99AC96EA8DFE}"/>
-    <hyperlink ref="C40" r:id="rId60" display="https://doi.org/10.31234/osf.io/mt49r" xr:uid="{9EA40F6E-B1C1-4A75-B481-39C90A03E75E}"/>
-    <hyperlink ref="C41" r:id="rId61" display="https://doi.org/10.31234/osf.io/bnsx2" xr:uid="{63D5CDF4-C3ED-4621-886B-026265E45F56}"/>
-    <hyperlink ref="E41" r:id="rId62" xr:uid="{08AABF7C-2FA2-46EF-98CF-56A84170523F}"/>
-    <hyperlink ref="C8" r:id="rId63" display="https://doi.org/10.1007/s41449-025-00460-x" xr:uid="{A0B3F658-F0ED-4C9D-BD5A-8C5E0B28DDAD}"/>
-    <hyperlink ref="E8" r:id="rId64" xr:uid="{86E48510-5694-4822-9C15-811C53298144}"/>
-    <hyperlink ref="F8" r:id="rId65" xr:uid="{F2CF54DC-82BB-4B77-9942-9BF93FA7F0A6}"/>
-    <hyperlink ref="G7" r:id="rId66" xr:uid="{C48C75DC-DB55-4450-A4F7-E9E0C34ECC15}"/>
-    <hyperlink ref="E6" r:id="rId67" xr:uid="{18606C55-07D2-45E4-8557-E96814F20E71}"/>
-    <hyperlink ref="G6" r:id="rId68" xr:uid="{080935E3-AB10-41DA-A9E4-594385CA18FB}"/>
-    <hyperlink ref="E5" r:id="rId69" xr:uid="{CD47EA21-01E5-4F81-861D-1BCF591E3D8D}"/>
-    <hyperlink ref="G5" r:id="rId70" xr:uid="{DB58B12E-C04C-4B6A-99CE-11EF593D3E0F}"/>
-    <hyperlink ref="C34" r:id="rId71" display="https://doi.org/10.31222/osf.io/8psw2" xr:uid="{C0F54102-918A-4578-B027-C78823FD4B7D}"/>
+    <hyperlink ref="E10" r:id="rId1" xr:uid="{41A1C6B5-F794-4E36-A76C-521B33FA2C7E}"/>
+    <hyperlink ref="F10" r:id="rId2" xr:uid="{D45BBE43-E931-4EDA-AB62-49ECCD4358D7}"/>
+    <hyperlink ref="C11" r:id="rId3" display="https://doi.org/10.5281/zenodo.13945051" xr:uid="{15B1DF19-42C9-4721-BDEE-790C2BD36401}"/>
+    <hyperlink ref="E11" r:id="rId4" xr:uid="{EE424F71-99CE-4EE2-B51B-A911BE1F8393}"/>
+    <hyperlink ref="G11" r:id="rId5" xr:uid="{3F25FBC9-AB32-4C97-9E08-65B039840DB8}"/>
+    <hyperlink ref="C12" r:id="rId6" display="https://doi.org/10.18718/81781.38" xr:uid="{782B69DE-8E85-4D8F-9DAC-8EB607F3F04E}"/>
+    <hyperlink ref="E12" r:id="rId7" xr:uid="{9A588C41-B2AF-4BF7-9A00-6DD9FB5CABFD}"/>
+    <hyperlink ref="F12" r:id="rId8" display="https://osf.io/8k9nt/" xr:uid="{159ED34F-FF9E-488E-B419-5DB75A1053A4}"/>
+    <hyperlink ref="C13" r:id="rId9" display="https://doi.org/10.15626/MP.2022.3236" xr:uid="{365B7B56-6668-4E66-B95F-686BDD31EEE7}"/>
+    <hyperlink ref="E13" r:id="rId10" xr:uid="{6F806BFE-1E43-477A-98D8-853E317AB860}"/>
+    <hyperlink ref="G13" r:id="rId11" xr:uid="{39191331-4837-4425-955D-F7F137894FA7}"/>
+    <hyperlink ref="E14" r:id="rId12" xr:uid="{BF2F029F-64B8-458D-9E6D-FB7B0A9D9E54}"/>
+    <hyperlink ref="G14" r:id="rId13" xr:uid="{130EB372-4CDB-40F4-B733-C289D48B1C4C}"/>
+    <hyperlink ref="C15" r:id="rId14" display="https://doi.org/10.15626/MP.2020.2639" xr:uid="{B96128B1-8C8B-4E74-8D94-6ECC038C9AAC}"/>
+    <hyperlink ref="E15" r:id="rId15" xr:uid="{AD4669E7-2751-41A0-BCE5-14632257828B}"/>
+    <hyperlink ref="G15" r:id="rId16" xr:uid="{3D2FC1C8-D1F7-407E-B397-D60D8B7AA2EA}"/>
+    <hyperlink ref="C16" r:id="rId17" display="https://doi.org/10.5334/jopd.92" xr:uid="{A071F59A-946C-461F-A4B7-033C6C45173A}"/>
+    <hyperlink ref="C17" r:id="rId18" display="https://doi.org/10.1016/j.jbusres.2023.114189" xr:uid="{51055E7B-DEE6-4A19-92E4-D1721DF822B1}"/>
+    <hyperlink ref="E17" r:id="rId19" xr:uid="{ED578A9E-FF99-4C7B-8A91-7C05D3B75022}"/>
+    <hyperlink ref="G17" r:id="rId20" xr:uid="{9BB5D8E7-F006-4255-8265-71EA7D3EBCE4}"/>
+    <hyperlink ref="C18" r:id="rId21" display="http://doi.org/10.5334/jopd.67" xr:uid="{C4050047-C1E1-404E-B073-E0C05CE8D173}"/>
+    <hyperlink ref="E18" r:id="rId22" xr:uid="{E3FEC74A-0F6F-4FFC-8AC0-B45670656896}"/>
+    <hyperlink ref="G18" r:id="rId23" xr:uid="{5C54A4BE-8B8C-494A-B29D-49F490A2C1C2}"/>
+    <hyperlink ref="C19" r:id="rId24" display="https://doi.org/10.1073/pnas.212037711" xr:uid="{C93D8067-4FC0-4D8D-8E47-D00FBE2F6608}"/>
+    <hyperlink ref="C20" r:id="rId25" display="https://doi.org/10.1037/bul0000356" xr:uid="{BDFC91BF-1233-4C67-A06A-DDE12D0F8BEB}"/>
+    <hyperlink ref="E20" r:id="rId26" xr:uid="{D92AA8D7-14D0-4433-B7CB-0E1DF9F275E9}"/>
+    <hyperlink ref="F20" r:id="rId27" xr:uid="{FB02A3AD-7B15-4C0E-9F16-631065DCF554}"/>
+    <hyperlink ref="C21" r:id="rId28" display="https://doi.org/10.1080/02699931.2021.1979473" xr:uid="{AD06D523-F5DB-442E-B989-A6C32B777ED1}"/>
+    <hyperlink ref="E21" r:id="rId29" xr:uid="{7BB9E6E9-A4CD-49AA-A55E-7BDA3DFBBEC0}"/>
+    <hyperlink ref="F21" r:id="rId30" xr:uid="{21E90428-3D65-4277-B80F-141F81A55916}"/>
+    <hyperlink ref="C22" r:id="rId31" display="https://doi.org/10.1016/j.jesp.2020.104066" xr:uid="{2A8C850C-91E2-46B0-987D-55EB0D9C3B0F}"/>
+    <hyperlink ref="E22" r:id="rId32" display="https://osf.io/96de2" xr:uid="{6C52A618-C82D-476C-89C8-16F20F642485}"/>
+    <hyperlink ref="C23" r:id="rId33" display="https://doi.org/10.5964/ejop.2639" xr:uid="{0DFC4B36-9C4B-4E2A-92F6-E6D628E09B18}"/>
+    <hyperlink ref="C24" r:id="rId34" display="https://doi.org/10.1177/1745691620984474" xr:uid="{54D1B1A1-B51A-4CA8-9C8A-8B2BF483FDDC}"/>
+    <hyperlink ref="C25" r:id="rId35" display="https://doi.org/10.1016/j.jesp.2020.104060" xr:uid="{862E7504-584A-4242-9B75-22375BC49E27}"/>
+    <hyperlink ref="C26" r:id="rId36" display="https://doi.org/10.1016/j.jesp.2019.103942" xr:uid="{B8F41347-13BD-4D71-A682-6BD22F709DE9}"/>
+    <hyperlink ref="C27" r:id="rId37" display="https://doi.org/10.1037/bul0000220" xr:uid="{065B9BF3-E67C-451C-B12A-2782BA816965}"/>
+    <hyperlink ref="G27" r:id="rId38" display="https://www.researchgate.net/publication/337261659_Crowdsourcing_Hypothesis_Tests_Making_Transparent_How_Design_Choices_Shape_Research_Results" xr:uid="{099DB906-00A3-4756-8332-B3B87A0D9EEF}"/>
+    <hyperlink ref="C28" r:id="rId39" display="https://osf.io/34sv6" xr:uid="{DD65BC2F-BFCE-4797-B982-DFEB045FD826}"/>
+    <hyperlink ref="G28" r:id="rId40" xr:uid="{87350DFD-AAFD-4459-9249-138523C66895}"/>
+    <hyperlink ref="C29" r:id="rId41" display="https://doi.org/10.31234/osf.io/akfzh" xr:uid="{9B39A2DF-F148-4367-8E24-E1AFFA69762A}"/>
+    <hyperlink ref="F29" r:id="rId42" xr:uid="{BACE566D-5B6D-4E9A-81EF-685F01A92950}"/>
+    <hyperlink ref="C30" r:id="rId43" display="https://doi.org/10.31234/osf.io/gj76p" xr:uid="{B34F1845-E395-44F6-9C3F-A1DC39394D59}"/>
+    <hyperlink ref="C31" r:id="rId44" display="https://doi.org/10.31234/osf.io/krwcn" xr:uid="{BEF8554E-090A-4B5A-89F1-432B57FC20C6}"/>
+    <hyperlink ref="G31" r:id="rId45" xr:uid="{5C9D188F-41F0-4255-9A7F-776DC0D7C6B3}"/>
+    <hyperlink ref="C32" r:id="rId46" display="https://osf.io/preprints/metaarxiv/ewb2t" xr:uid="{73F38CDC-AE74-42AE-9875-B80E70CAAD04}"/>
+    <hyperlink ref="G32" r:id="rId47" xr:uid="{F242B96D-FDF5-4CE7-BDFB-CFE6A00240A0}"/>
+    <hyperlink ref="C33" r:id="rId48" display="https://osf.io/8cwpy" xr:uid="{092A1365-FCB4-41FB-8313-CF735B66A2DD}"/>
+    <hyperlink ref="E33" r:id="rId49" xr:uid="{ECBA28D3-FB1C-4193-901B-41108340BCFD}"/>
+    <hyperlink ref="F33" r:id="rId50" display="https://osf.io/c2ynz" xr:uid="{E93BA08A-3A49-4D35-AC66-D74574AF96C4}"/>
+    <hyperlink ref="F35" r:id="rId51" xr:uid="{97ACEB9A-0C43-4AA2-ACFE-F50A4B6B56F0}"/>
+    <hyperlink ref="C36" r:id="rId52" display="https://doi.org/10.31234/osf.io/2kfh3" xr:uid="{FE4142A2-4633-4F53-8F23-5F50CB46E97C}"/>
+    <hyperlink ref="F36" r:id="rId53" xr:uid="{174B565C-80A9-4205-A2B1-E2DC35E916D7}"/>
+    <hyperlink ref="C37" r:id="rId54" display="https://doi.org/10.31234/osf.io/ntukz" xr:uid="{562912E7-E3CF-4637-A5EC-F5598C18FAED}"/>
+    <hyperlink ref="F37" r:id="rId55" display="https://osf.io/7pw4c/" xr:uid="{E5872E1A-19BD-48E3-BBC5-0325DE4F50E7}"/>
+    <hyperlink ref="C38" r:id="rId56" display="https://doi.org/10.31234/osf.io/wf2tn" xr:uid="{A453771E-19D2-48CD-8D51-59EE29E521DB}"/>
+    <hyperlink ref="C39" r:id="rId57" display="https://doi.org/10.31219/osf.io/2tr6q" xr:uid="{0F998EE8-1C6C-4120-A8A7-D2F043592BCD}"/>
+    <hyperlink ref="F39" r:id="rId58" display="https://osf.io/9qz3d" xr:uid="{4BBBB1B2-2501-4EEF-8BB3-87C7A2170367}"/>
+    <hyperlink ref="C40" r:id="rId59" display="https://doi.org/10.31234/osf.io/hjbwp" xr:uid="{519680D7-CB35-4C47-AB82-99AC96EA8DFE}"/>
+    <hyperlink ref="C41" r:id="rId60" display="https://doi.org/10.31234/osf.io/mt49r" xr:uid="{9EA40F6E-B1C1-4A75-B481-39C90A03E75E}"/>
+    <hyperlink ref="C42" r:id="rId61" display="https://doi.org/10.31234/osf.io/bnsx2" xr:uid="{63D5CDF4-C3ED-4621-886B-026265E45F56}"/>
+    <hyperlink ref="E42" r:id="rId62" xr:uid="{08AABF7C-2FA2-46EF-98CF-56A84170523F}"/>
+    <hyperlink ref="C9" r:id="rId63" display="https://doi.org/10.1007/s41449-025-00460-x" xr:uid="{A0B3F658-F0ED-4C9D-BD5A-8C5E0B28DDAD}"/>
+    <hyperlink ref="E9" r:id="rId64" xr:uid="{86E48510-5694-4822-9C15-811C53298144}"/>
+    <hyperlink ref="F9" r:id="rId65" xr:uid="{F2CF54DC-82BB-4B77-9942-9BF93FA7F0A6}"/>
+    <hyperlink ref="G8" r:id="rId66" xr:uid="{C48C75DC-DB55-4450-A4F7-E9E0C34ECC15}"/>
+    <hyperlink ref="E7" r:id="rId67" xr:uid="{18606C55-07D2-45E4-8557-E96814F20E71}"/>
+    <hyperlink ref="G7" r:id="rId68" xr:uid="{080935E3-AB10-41DA-A9E4-594385CA18FB}"/>
+    <hyperlink ref="E6" r:id="rId69" xr:uid="{CD47EA21-01E5-4F81-861D-1BCF591E3D8D}"/>
+    <hyperlink ref="G6" r:id="rId70" xr:uid="{DB58B12E-C04C-4B6A-99CE-11EF593D3E0F}"/>
+    <hyperlink ref="C35" r:id="rId71" display="https://doi.org/10.31222/osf.io/8psw2" xr:uid="{C0F54102-918A-4578-B027-C78823FD4B7D}"/>
+    <hyperlink ref="G3" r:id="rId72" xr:uid="{5DE4B276-23A0-4D61-A9EA-3B94D7A67DC6}"/>
+    <hyperlink ref="G4" r:id="rId73" xr:uid="{BE4A9D01-B112-43BD-92AC-389201076D3D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId72"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId74"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removed duplicate (R2 description) and updated "No Room at the Inn"
</commit_message>
<xml_diff>
--- a/research.xlsx
+++ b/research.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lroesele.IVV5NET\sciebo - Röseler, Lukas (lroesele@uni-muenster.de)@uni-muenster.sciebo.de\LeaRn\home\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C773C9B6-7E09-4C9A-A504-0B76C34582DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2505BD79-573D-4758-8C1F-38D76CF2D8A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AAC91D46-EE41-4CEB-9A66-251368506452}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{AAC91D46-EE41-4CEB-9A66-251368506452}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="152">
   <si>
     <t>#</t>
   </si>
@@ -754,6 +754,9 @@
   </si>
   <si>
     <t>https://doi.org/10.5281/zenodo.17279413</t>
+  </si>
+  <si>
+    <t>Gold (APC: 3060 USD)</t>
   </si>
 </sst>
 </file>
@@ -1200,7 +1203,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1381,7 +1384,7 @@
         <v>136</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>

</xml_diff>

<commit_message>
Added publication, created new section for editorial activities, added toc, new render
</commit_message>
<xml_diff>
--- a/research.xlsx
+++ b/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lroesele.IVV5NET\sciebo - Röseler, Lukas (lroesele@uni-muenster.de)@uni-muenster.sciebo.de\LeaRn\home\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2505BD79-573D-4758-8C1F-38D76CF2D8A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB1B263-1967-419E-869A-317AF8837D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{AAC91D46-EE41-4CEB-9A66-251368506452}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="155">
   <si>
     <t>#</t>
   </si>
@@ -757,6 +757,38 @@
   </si>
   <si>
     <t>Gold (APC: 3060 USD)</t>
+  </si>
+  <si>
+    <t>Publishing</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Müller, M., </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Röseler, L.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, &amp; Wallrich, L. (2025). Initial Editorial Assessment Form (Replication Research) (1.0). Zenodo. https://doi.org/10.5281/zenodo.17911973</t>
+    </r>
+  </si>
+  <si>
+    <t>https://doi.org/10.5281/zenodo.17911973</t>
   </si>
 </sst>
 </file>
@@ -1200,10 +1232,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D3A1534-13D7-4FF4-8CD6-0F369116C1B6}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1239,43 +1271,47 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>41</v>
+        <v>152</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
-        <v>148</v>
+      <c r="E2" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>154</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>146</v>
+        <v>41</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>147</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>140</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="9" t="s">
-        <v>149</v>
+      <c r="G3" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>10</v>
@@ -1283,13 +1319,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>140</v>
@@ -1297,221 +1333,219 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>37</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>36</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="H6" s="2" t="s">
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>140</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="F7" s="9"/>
+        <v>141</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>142</v>
+      </c>
       <c r="G7" s="11" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="E8" s="9"/>
+        <v>140</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>137</v>
+      </c>
       <c r="F8" s="9"/>
       <c r="G8" s="11" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="1"/>
+        <v>151</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="11" t="s">
+        <v>134</v>
+      </c>
       <c r="H9" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="7"/>
+      <c r="G10" s="1"/>
       <c r="H10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
+        <v>32</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="7"/>
+      <c r="H11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>31</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="4" t="s">
+      <c r="F12" s="7"/>
+      <c r="G12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="H12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>30</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>29</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>20</v>
@@ -1519,23 +1553,23 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>122</v>
+        <v>21</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>20</v>
@@ -1543,23 +1577,23 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>122</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>20</v>
@@ -1567,25 +1601,23 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>34</v>
+        <v>19</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="G16" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>20</v>
@@ -1593,91 +1625,93 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>28</v>
+        <v>37</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="4" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
+        <v>24</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="7"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
+      <c r="G19" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="H19" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>47</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="2" t="s">
         <v>10</v>
@@ -1685,67 +1719,71 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G21" s="7"/>
       <c r="H21" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>123</v>
+        <v>49</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="G22" s="7"/>
       <c r="H22" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>19</v>
-      </c>
       <c r="B23" s="2" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
+        <v>51</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>123</v>
+      </c>
       <c r="G23" s="7"/>
       <c r="H23" s="2" t="s">
         <v>20</v>
@@ -1753,46 +1791,42 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="G25" s="7"/>
       <c r="H25" s="2" t="s">
@@ -1801,22 +1835,22 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>9</v>
+        <v>57</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G26" s="7"/>
       <c r="H26" s="2" t="s">
@@ -1825,49 +1859,49 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>68</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="G27" s="7"/>
       <c r="H27" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>19</v>
+        <v>65</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F28" s="7"/>
+        <v>66</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="G28" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>10</v>
@@ -1875,25 +1909,23 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>140</v>
+        <v>19</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
+      </c>
+      <c r="F29" s="7"/>
+      <c r="G29" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>10</v>
@@ -1901,23 +1933,25 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>140</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F30" s="7"/>
+        <v>74</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="G30" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>10</v>
@@ -1925,25 +1959,23 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>77</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>140</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
+      </c>
+      <c r="F31" s="7"/>
+      <c r="G31" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>10</v>
@@ -1951,363 +1983,391 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>140</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F32" s="7"/>
+        <v>34</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="G32" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E33" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>88</v>
+      <c r="E33" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F33" s="7"/>
+      <c r="G33" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>90</v>
+        <v>21</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>34</v>
+      <c r="E34" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>124</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>93</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>140</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>96</v>
+        <v>91</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>20</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>131</v>
+        <v>94</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>19</v>
+        <v>140</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
+        <v>7</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
         <v>6</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
-        <v>5</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>140</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F38" s="7"/>
+        <v>102</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>125</v>
+      </c>
       <c r="G38" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>140</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>126</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="F39" s="7"/>
       <c r="G39" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>140</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>127</v>
+        <v>108</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>140</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>34</v>
+        <v>111</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>127</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>116</v>
+        <v>41</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>1</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E43" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="G43" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="H43" s="2" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E10" r:id="rId1" xr:uid="{41A1C6B5-F794-4E36-A76C-521B33FA2C7E}"/>
-    <hyperlink ref="F10" r:id="rId2" xr:uid="{D45BBE43-E931-4EDA-AB62-49ECCD4358D7}"/>
-    <hyperlink ref="C11" r:id="rId3" display="https://doi.org/10.5281/zenodo.13945051" xr:uid="{15B1DF19-42C9-4721-BDEE-790C2BD36401}"/>
-    <hyperlink ref="E11" r:id="rId4" xr:uid="{EE424F71-99CE-4EE2-B51B-A911BE1F8393}"/>
-    <hyperlink ref="G11" r:id="rId5" xr:uid="{3F25FBC9-AB32-4C97-9E08-65B039840DB8}"/>
-    <hyperlink ref="C12" r:id="rId6" display="https://doi.org/10.18718/81781.38" xr:uid="{782B69DE-8E85-4D8F-9DAC-8EB607F3F04E}"/>
-    <hyperlink ref="E12" r:id="rId7" xr:uid="{9A588C41-B2AF-4BF7-9A00-6DD9FB5CABFD}"/>
-    <hyperlink ref="F12" r:id="rId8" display="https://osf.io/8k9nt/" xr:uid="{159ED34F-FF9E-488E-B419-5DB75A1053A4}"/>
-    <hyperlink ref="C13" r:id="rId9" display="https://doi.org/10.15626/MP.2022.3236" xr:uid="{365B7B56-6668-4E66-B95F-686BDD31EEE7}"/>
-    <hyperlink ref="E13" r:id="rId10" xr:uid="{6F806BFE-1E43-477A-98D8-853E317AB860}"/>
-    <hyperlink ref="G13" r:id="rId11" xr:uid="{39191331-4837-4425-955D-F7F137894FA7}"/>
-    <hyperlink ref="E14" r:id="rId12" xr:uid="{BF2F029F-64B8-458D-9E6D-FB7B0A9D9E54}"/>
-    <hyperlink ref="G14" r:id="rId13" xr:uid="{130EB372-4CDB-40F4-B733-C289D48B1C4C}"/>
-    <hyperlink ref="C15" r:id="rId14" display="https://doi.org/10.15626/MP.2020.2639" xr:uid="{B96128B1-8C8B-4E74-8D94-6ECC038C9AAC}"/>
-    <hyperlink ref="E15" r:id="rId15" xr:uid="{AD4669E7-2751-41A0-BCE5-14632257828B}"/>
-    <hyperlink ref="G15" r:id="rId16" xr:uid="{3D2FC1C8-D1F7-407E-B397-D60D8B7AA2EA}"/>
-    <hyperlink ref="C16" r:id="rId17" display="https://doi.org/10.5334/jopd.92" xr:uid="{A071F59A-946C-461F-A4B7-033C6C45173A}"/>
-    <hyperlink ref="C17" r:id="rId18" display="https://doi.org/10.1016/j.jbusres.2023.114189" xr:uid="{51055E7B-DEE6-4A19-92E4-D1721DF822B1}"/>
-    <hyperlink ref="E17" r:id="rId19" xr:uid="{ED578A9E-FF99-4C7B-8A91-7C05D3B75022}"/>
-    <hyperlink ref="G17" r:id="rId20" xr:uid="{9BB5D8E7-F006-4255-8265-71EA7D3EBCE4}"/>
-    <hyperlink ref="C18" r:id="rId21" display="http://doi.org/10.5334/jopd.67" xr:uid="{C4050047-C1E1-404E-B073-E0C05CE8D173}"/>
-    <hyperlink ref="E18" r:id="rId22" xr:uid="{E3FEC74A-0F6F-4FFC-8AC0-B45670656896}"/>
-    <hyperlink ref="G18" r:id="rId23" xr:uid="{5C54A4BE-8B8C-494A-B29D-49F490A2C1C2}"/>
-    <hyperlink ref="C19" r:id="rId24" display="https://doi.org/10.1073/pnas.212037711" xr:uid="{C93D8067-4FC0-4D8D-8E47-D00FBE2F6608}"/>
-    <hyperlink ref="C20" r:id="rId25" display="https://doi.org/10.1037/bul0000356" xr:uid="{BDFC91BF-1233-4C67-A06A-DDE12D0F8BEB}"/>
-    <hyperlink ref="E20" r:id="rId26" xr:uid="{D92AA8D7-14D0-4433-B7CB-0E1DF9F275E9}"/>
-    <hyperlink ref="F20" r:id="rId27" xr:uid="{FB02A3AD-7B15-4C0E-9F16-631065DCF554}"/>
-    <hyperlink ref="C21" r:id="rId28" display="https://doi.org/10.1080/02699931.2021.1979473" xr:uid="{AD06D523-F5DB-442E-B989-A6C32B777ED1}"/>
-    <hyperlink ref="E21" r:id="rId29" xr:uid="{7BB9E6E9-A4CD-49AA-A55E-7BDA3DFBBEC0}"/>
-    <hyperlink ref="F21" r:id="rId30" xr:uid="{21E90428-3D65-4277-B80F-141F81A55916}"/>
-    <hyperlink ref="C22" r:id="rId31" display="https://doi.org/10.1016/j.jesp.2020.104066" xr:uid="{2A8C850C-91E2-46B0-987D-55EB0D9C3B0F}"/>
-    <hyperlink ref="E22" r:id="rId32" display="https://osf.io/96de2" xr:uid="{6C52A618-C82D-476C-89C8-16F20F642485}"/>
-    <hyperlink ref="C23" r:id="rId33" display="https://doi.org/10.5964/ejop.2639" xr:uid="{0DFC4B36-9C4B-4E2A-92F6-E6D628E09B18}"/>
-    <hyperlink ref="C24" r:id="rId34" display="https://doi.org/10.1177/1745691620984474" xr:uid="{54D1B1A1-B51A-4CA8-9C8A-8B2BF483FDDC}"/>
-    <hyperlink ref="C25" r:id="rId35" display="https://doi.org/10.1016/j.jesp.2020.104060" xr:uid="{862E7504-584A-4242-9B75-22375BC49E27}"/>
-    <hyperlink ref="C26" r:id="rId36" display="https://doi.org/10.1016/j.jesp.2019.103942" xr:uid="{B8F41347-13BD-4D71-A682-6BD22F709DE9}"/>
-    <hyperlink ref="C27" r:id="rId37" display="https://doi.org/10.1037/bul0000220" xr:uid="{065B9BF3-E67C-451C-B12A-2782BA816965}"/>
-    <hyperlink ref="G27" r:id="rId38" display="https://www.researchgate.net/publication/337261659_Crowdsourcing_Hypothesis_Tests_Making_Transparent_How_Design_Choices_Shape_Research_Results" xr:uid="{099DB906-00A3-4756-8332-B3B87A0D9EEF}"/>
-    <hyperlink ref="C28" r:id="rId39" display="https://osf.io/34sv6" xr:uid="{DD65BC2F-BFCE-4797-B982-DFEB045FD826}"/>
-    <hyperlink ref="G28" r:id="rId40" xr:uid="{87350DFD-AAFD-4459-9249-138523C66895}"/>
-    <hyperlink ref="C29" r:id="rId41" display="https://doi.org/10.31234/osf.io/akfzh" xr:uid="{9B39A2DF-F148-4367-8E24-E1AFFA69762A}"/>
-    <hyperlink ref="F29" r:id="rId42" xr:uid="{BACE566D-5B6D-4E9A-81EF-685F01A92950}"/>
-    <hyperlink ref="C30" r:id="rId43" display="https://doi.org/10.31234/osf.io/gj76p" xr:uid="{B34F1845-E395-44F6-9C3F-A1DC39394D59}"/>
-    <hyperlink ref="C31" r:id="rId44" display="https://doi.org/10.31234/osf.io/krwcn" xr:uid="{BEF8554E-090A-4B5A-89F1-432B57FC20C6}"/>
-    <hyperlink ref="G31" r:id="rId45" xr:uid="{5C9D188F-41F0-4255-9A7F-776DC0D7C6B3}"/>
-    <hyperlink ref="C32" r:id="rId46" display="https://osf.io/preprints/metaarxiv/ewb2t" xr:uid="{73F38CDC-AE74-42AE-9875-B80E70CAAD04}"/>
-    <hyperlink ref="G32" r:id="rId47" xr:uid="{F242B96D-FDF5-4CE7-BDFB-CFE6A00240A0}"/>
-    <hyperlink ref="C33" r:id="rId48" display="https://osf.io/8cwpy" xr:uid="{092A1365-FCB4-41FB-8313-CF735B66A2DD}"/>
-    <hyperlink ref="E33" r:id="rId49" xr:uid="{ECBA28D3-FB1C-4193-901B-41108340BCFD}"/>
-    <hyperlink ref="F33" r:id="rId50" display="https://osf.io/c2ynz" xr:uid="{E93BA08A-3A49-4D35-AC66-D74574AF96C4}"/>
-    <hyperlink ref="F35" r:id="rId51" xr:uid="{97ACEB9A-0C43-4AA2-ACFE-F50A4B6B56F0}"/>
-    <hyperlink ref="C36" r:id="rId52" display="https://doi.org/10.31234/osf.io/2kfh3" xr:uid="{FE4142A2-4633-4F53-8F23-5F50CB46E97C}"/>
-    <hyperlink ref="F36" r:id="rId53" xr:uid="{174B565C-80A9-4205-A2B1-E2DC35E916D7}"/>
-    <hyperlink ref="C37" r:id="rId54" display="https://doi.org/10.31234/osf.io/ntukz" xr:uid="{562912E7-E3CF-4637-A5EC-F5598C18FAED}"/>
-    <hyperlink ref="F37" r:id="rId55" display="https://osf.io/7pw4c/" xr:uid="{E5872E1A-19BD-48E3-BBC5-0325DE4F50E7}"/>
-    <hyperlink ref="C38" r:id="rId56" display="https://doi.org/10.31234/osf.io/wf2tn" xr:uid="{A453771E-19D2-48CD-8D51-59EE29E521DB}"/>
-    <hyperlink ref="C39" r:id="rId57" display="https://doi.org/10.31219/osf.io/2tr6q" xr:uid="{0F998EE8-1C6C-4120-A8A7-D2F043592BCD}"/>
-    <hyperlink ref="F39" r:id="rId58" display="https://osf.io/9qz3d" xr:uid="{4BBBB1B2-2501-4EEF-8BB3-87C7A2170367}"/>
-    <hyperlink ref="C40" r:id="rId59" display="https://doi.org/10.31234/osf.io/hjbwp" xr:uid="{519680D7-CB35-4C47-AB82-99AC96EA8DFE}"/>
-    <hyperlink ref="C41" r:id="rId60" display="https://doi.org/10.31234/osf.io/mt49r" xr:uid="{9EA40F6E-B1C1-4A75-B481-39C90A03E75E}"/>
-    <hyperlink ref="C42" r:id="rId61" display="https://doi.org/10.31234/osf.io/bnsx2" xr:uid="{63D5CDF4-C3ED-4621-886B-026265E45F56}"/>
-    <hyperlink ref="E42" r:id="rId62" xr:uid="{08AABF7C-2FA2-46EF-98CF-56A84170523F}"/>
-    <hyperlink ref="C9" r:id="rId63" display="https://doi.org/10.1007/s41449-025-00460-x" xr:uid="{A0B3F658-F0ED-4C9D-BD5A-8C5E0B28DDAD}"/>
-    <hyperlink ref="E9" r:id="rId64" xr:uid="{86E48510-5694-4822-9C15-811C53298144}"/>
-    <hyperlink ref="F9" r:id="rId65" xr:uid="{F2CF54DC-82BB-4B77-9942-9BF93FA7F0A6}"/>
-    <hyperlink ref="G8" r:id="rId66" xr:uid="{C48C75DC-DB55-4450-A4F7-E9E0C34ECC15}"/>
-    <hyperlink ref="E7" r:id="rId67" xr:uid="{18606C55-07D2-45E4-8557-E96814F20E71}"/>
-    <hyperlink ref="G7" r:id="rId68" xr:uid="{080935E3-AB10-41DA-A9E4-594385CA18FB}"/>
-    <hyperlink ref="E6" r:id="rId69" xr:uid="{CD47EA21-01E5-4F81-861D-1BCF591E3D8D}"/>
-    <hyperlink ref="G6" r:id="rId70" xr:uid="{DB58B12E-C04C-4B6A-99CE-11EF593D3E0F}"/>
-    <hyperlink ref="C35" r:id="rId71" display="https://doi.org/10.31222/osf.io/8psw2" xr:uid="{C0F54102-918A-4578-B027-C78823FD4B7D}"/>
-    <hyperlink ref="G3" r:id="rId72" xr:uid="{5DE4B276-23A0-4D61-A9EA-3B94D7A67DC6}"/>
-    <hyperlink ref="G4" r:id="rId73" xr:uid="{BE4A9D01-B112-43BD-92AC-389201076D3D}"/>
+    <hyperlink ref="E11" r:id="rId1" xr:uid="{41A1C6B5-F794-4E36-A76C-521B33FA2C7E}"/>
+    <hyperlink ref="F11" r:id="rId2" xr:uid="{D45BBE43-E931-4EDA-AB62-49ECCD4358D7}"/>
+    <hyperlink ref="C12" r:id="rId3" display="https://doi.org/10.5281/zenodo.13945051" xr:uid="{15B1DF19-42C9-4721-BDEE-790C2BD36401}"/>
+    <hyperlink ref="E12" r:id="rId4" xr:uid="{EE424F71-99CE-4EE2-B51B-A911BE1F8393}"/>
+    <hyperlink ref="G12" r:id="rId5" xr:uid="{3F25FBC9-AB32-4C97-9E08-65B039840DB8}"/>
+    <hyperlink ref="C13" r:id="rId6" display="https://doi.org/10.18718/81781.38" xr:uid="{782B69DE-8E85-4D8F-9DAC-8EB607F3F04E}"/>
+    <hyperlink ref="E13" r:id="rId7" xr:uid="{9A588C41-B2AF-4BF7-9A00-6DD9FB5CABFD}"/>
+    <hyperlink ref="F13" r:id="rId8" display="https://osf.io/8k9nt/" xr:uid="{159ED34F-FF9E-488E-B419-5DB75A1053A4}"/>
+    <hyperlink ref="C14" r:id="rId9" display="https://doi.org/10.15626/MP.2022.3236" xr:uid="{365B7B56-6668-4E66-B95F-686BDD31EEE7}"/>
+    <hyperlink ref="E14" r:id="rId10" xr:uid="{6F806BFE-1E43-477A-98D8-853E317AB860}"/>
+    <hyperlink ref="G14" r:id="rId11" xr:uid="{39191331-4837-4425-955D-F7F137894FA7}"/>
+    <hyperlink ref="E15" r:id="rId12" xr:uid="{BF2F029F-64B8-458D-9E6D-FB7B0A9D9E54}"/>
+    <hyperlink ref="G15" r:id="rId13" xr:uid="{130EB372-4CDB-40F4-B733-C289D48B1C4C}"/>
+    <hyperlink ref="C16" r:id="rId14" display="https://doi.org/10.15626/MP.2020.2639" xr:uid="{B96128B1-8C8B-4E74-8D94-6ECC038C9AAC}"/>
+    <hyperlink ref="E16" r:id="rId15" xr:uid="{AD4669E7-2751-41A0-BCE5-14632257828B}"/>
+    <hyperlink ref="G16" r:id="rId16" xr:uid="{3D2FC1C8-D1F7-407E-B397-D60D8B7AA2EA}"/>
+    <hyperlink ref="C17" r:id="rId17" display="https://doi.org/10.5334/jopd.92" xr:uid="{A071F59A-946C-461F-A4B7-033C6C45173A}"/>
+    <hyperlink ref="C18" r:id="rId18" display="https://doi.org/10.1016/j.jbusres.2023.114189" xr:uid="{51055E7B-DEE6-4A19-92E4-D1721DF822B1}"/>
+    <hyperlink ref="E18" r:id="rId19" xr:uid="{ED578A9E-FF99-4C7B-8A91-7C05D3B75022}"/>
+    <hyperlink ref="G18" r:id="rId20" xr:uid="{9BB5D8E7-F006-4255-8265-71EA7D3EBCE4}"/>
+    <hyperlink ref="C19" r:id="rId21" display="http://doi.org/10.5334/jopd.67" xr:uid="{C4050047-C1E1-404E-B073-E0C05CE8D173}"/>
+    <hyperlink ref="E19" r:id="rId22" xr:uid="{E3FEC74A-0F6F-4FFC-8AC0-B45670656896}"/>
+    <hyperlink ref="G19" r:id="rId23" xr:uid="{5C54A4BE-8B8C-494A-B29D-49F490A2C1C2}"/>
+    <hyperlink ref="C20" r:id="rId24" display="https://doi.org/10.1073/pnas.212037711" xr:uid="{C93D8067-4FC0-4D8D-8E47-D00FBE2F6608}"/>
+    <hyperlink ref="C21" r:id="rId25" display="https://doi.org/10.1037/bul0000356" xr:uid="{BDFC91BF-1233-4C67-A06A-DDE12D0F8BEB}"/>
+    <hyperlink ref="E21" r:id="rId26" xr:uid="{D92AA8D7-14D0-4433-B7CB-0E1DF9F275E9}"/>
+    <hyperlink ref="F21" r:id="rId27" xr:uid="{FB02A3AD-7B15-4C0E-9F16-631065DCF554}"/>
+    <hyperlink ref="C22" r:id="rId28" display="https://doi.org/10.1080/02699931.2021.1979473" xr:uid="{AD06D523-F5DB-442E-B989-A6C32B777ED1}"/>
+    <hyperlink ref="E22" r:id="rId29" xr:uid="{7BB9E6E9-A4CD-49AA-A55E-7BDA3DFBBEC0}"/>
+    <hyperlink ref="F22" r:id="rId30" xr:uid="{21E90428-3D65-4277-B80F-141F81A55916}"/>
+    <hyperlink ref="C23" r:id="rId31" display="https://doi.org/10.1016/j.jesp.2020.104066" xr:uid="{2A8C850C-91E2-46B0-987D-55EB0D9C3B0F}"/>
+    <hyperlink ref="E23" r:id="rId32" display="https://osf.io/96de2" xr:uid="{6C52A618-C82D-476C-89C8-16F20F642485}"/>
+    <hyperlink ref="C24" r:id="rId33" display="https://doi.org/10.5964/ejop.2639" xr:uid="{0DFC4B36-9C4B-4E2A-92F6-E6D628E09B18}"/>
+    <hyperlink ref="C25" r:id="rId34" display="https://doi.org/10.1177/1745691620984474" xr:uid="{54D1B1A1-B51A-4CA8-9C8A-8B2BF483FDDC}"/>
+    <hyperlink ref="C26" r:id="rId35" display="https://doi.org/10.1016/j.jesp.2020.104060" xr:uid="{862E7504-584A-4242-9B75-22375BC49E27}"/>
+    <hyperlink ref="C27" r:id="rId36" display="https://doi.org/10.1016/j.jesp.2019.103942" xr:uid="{B8F41347-13BD-4D71-A682-6BD22F709DE9}"/>
+    <hyperlink ref="C28" r:id="rId37" display="https://doi.org/10.1037/bul0000220" xr:uid="{065B9BF3-E67C-451C-B12A-2782BA816965}"/>
+    <hyperlink ref="G28" r:id="rId38" display="https://www.researchgate.net/publication/337261659_Crowdsourcing_Hypothesis_Tests_Making_Transparent_How_Design_Choices_Shape_Research_Results" xr:uid="{099DB906-00A3-4756-8332-B3B87A0D9EEF}"/>
+    <hyperlink ref="C29" r:id="rId39" display="https://osf.io/34sv6" xr:uid="{DD65BC2F-BFCE-4797-B982-DFEB045FD826}"/>
+    <hyperlink ref="G29" r:id="rId40" xr:uid="{87350DFD-AAFD-4459-9249-138523C66895}"/>
+    <hyperlink ref="C30" r:id="rId41" display="https://doi.org/10.31234/osf.io/akfzh" xr:uid="{9B39A2DF-F148-4367-8E24-E1AFFA69762A}"/>
+    <hyperlink ref="F30" r:id="rId42" xr:uid="{BACE566D-5B6D-4E9A-81EF-685F01A92950}"/>
+    <hyperlink ref="C31" r:id="rId43" display="https://doi.org/10.31234/osf.io/gj76p" xr:uid="{B34F1845-E395-44F6-9C3F-A1DC39394D59}"/>
+    <hyperlink ref="C32" r:id="rId44" display="https://doi.org/10.31234/osf.io/krwcn" xr:uid="{BEF8554E-090A-4B5A-89F1-432B57FC20C6}"/>
+    <hyperlink ref="G32" r:id="rId45" xr:uid="{5C9D188F-41F0-4255-9A7F-776DC0D7C6B3}"/>
+    <hyperlink ref="C33" r:id="rId46" display="https://osf.io/preprints/metaarxiv/ewb2t" xr:uid="{73F38CDC-AE74-42AE-9875-B80E70CAAD04}"/>
+    <hyperlink ref="G33" r:id="rId47" xr:uid="{F242B96D-FDF5-4CE7-BDFB-CFE6A00240A0}"/>
+    <hyperlink ref="C34" r:id="rId48" display="https://osf.io/8cwpy" xr:uid="{092A1365-FCB4-41FB-8313-CF735B66A2DD}"/>
+    <hyperlink ref="E34" r:id="rId49" xr:uid="{ECBA28D3-FB1C-4193-901B-41108340BCFD}"/>
+    <hyperlink ref="F34" r:id="rId50" display="https://osf.io/c2ynz" xr:uid="{E93BA08A-3A49-4D35-AC66-D74574AF96C4}"/>
+    <hyperlink ref="F36" r:id="rId51" xr:uid="{97ACEB9A-0C43-4AA2-ACFE-F50A4B6B56F0}"/>
+    <hyperlink ref="C37" r:id="rId52" display="https://doi.org/10.31234/osf.io/2kfh3" xr:uid="{FE4142A2-4633-4F53-8F23-5F50CB46E97C}"/>
+    <hyperlink ref="F37" r:id="rId53" xr:uid="{174B565C-80A9-4205-A2B1-E2DC35E916D7}"/>
+    <hyperlink ref="C38" r:id="rId54" display="https://doi.org/10.31234/osf.io/ntukz" xr:uid="{562912E7-E3CF-4637-A5EC-F5598C18FAED}"/>
+    <hyperlink ref="F38" r:id="rId55" display="https://osf.io/7pw4c/" xr:uid="{E5872E1A-19BD-48E3-BBC5-0325DE4F50E7}"/>
+    <hyperlink ref="C39" r:id="rId56" display="https://doi.org/10.31234/osf.io/wf2tn" xr:uid="{A453771E-19D2-48CD-8D51-59EE29E521DB}"/>
+    <hyperlink ref="C40" r:id="rId57" display="https://doi.org/10.31219/osf.io/2tr6q" xr:uid="{0F998EE8-1C6C-4120-A8A7-D2F043592BCD}"/>
+    <hyperlink ref="F40" r:id="rId58" display="https://osf.io/9qz3d" xr:uid="{4BBBB1B2-2501-4EEF-8BB3-87C7A2170367}"/>
+    <hyperlink ref="C41" r:id="rId59" display="https://doi.org/10.31234/osf.io/hjbwp" xr:uid="{519680D7-CB35-4C47-AB82-99AC96EA8DFE}"/>
+    <hyperlink ref="C42" r:id="rId60" display="https://doi.org/10.31234/osf.io/mt49r" xr:uid="{9EA40F6E-B1C1-4A75-B481-39C90A03E75E}"/>
+    <hyperlink ref="C43" r:id="rId61" display="https://doi.org/10.31234/osf.io/bnsx2" xr:uid="{63D5CDF4-C3ED-4621-886B-026265E45F56}"/>
+    <hyperlink ref="E43" r:id="rId62" xr:uid="{08AABF7C-2FA2-46EF-98CF-56A84170523F}"/>
+    <hyperlink ref="C10" r:id="rId63" display="https://doi.org/10.1007/s41449-025-00460-x" xr:uid="{A0B3F658-F0ED-4C9D-BD5A-8C5E0B28DDAD}"/>
+    <hyperlink ref="E10" r:id="rId64" xr:uid="{86E48510-5694-4822-9C15-811C53298144}"/>
+    <hyperlink ref="F10" r:id="rId65" xr:uid="{F2CF54DC-82BB-4B77-9942-9BF93FA7F0A6}"/>
+    <hyperlink ref="G9" r:id="rId66" xr:uid="{C48C75DC-DB55-4450-A4F7-E9E0C34ECC15}"/>
+    <hyperlink ref="E8" r:id="rId67" xr:uid="{18606C55-07D2-45E4-8557-E96814F20E71}"/>
+    <hyperlink ref="G8" r:id="rId68" xr:uid="{080935E3-AB10-41DA-A9E4-594385CA18FB}"/>
+    <hyperlink ref="E7" r:id="rId69" xr:uid="{CD47EA21-01E5-4F81-861D-1BCF591E3D8D}"/>
+    <hyperlink ref="G7" r:id="rId70" xr:uid="{DB58B12E-C04C-4B6A-99CE-11EF593D3E0F}"/>
+    <hyperlink ref="C36" r:id="rId71" display="https://doi.org/10.31222/osf.io/8psw2" xr:uid="{C0F54102-918A-4578-B027-C78823FD4B7D}"/>
+    <hyperlink ref="G4" r:id="rId72" xr:uid="{5DE4B276-23A0-4D61-A9EA-3B94D7A67DC6}"/>
+    <hyperlink ref="G5" r:id="rId73" xr:uid="{BE4A9D01-B112-43BD-92AC-389201076D3D}"/>
+    <hyperlink ref="E2" r:id="rId74" xr:uid="{BB6A0972-5774-4DF6-9260-A4734EF849A6}"/>
+    <hyperlink ref="G2" r:id="rId75" xr:uid="{99636F1B-E320-48F1-BD31-8C83856946A1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId74"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId76"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New render, added new paper
</commit_message>
<xml_diff>
--- a/research.xlsx
+++ b/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lroesele.IVV5NET\sciebo - Röseler, Lukas (lroesele@uni-muenster.de)@uni-muenster.sciebo.de\LeaRn\home\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB1B263-1967-419E-869A-317AF8837D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412D610C-680F-4FF9-A910-CAE9879EE444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{AAC91D46-EE41-4CEB-9A66-251368506452}"/>
   </bookViews>
@@ -341,9 +341,6 @@
     <t>https://osf.io/preprints/metaarxiv/ewb2t</t>
   </si>
   <si>
-    <t>Röseler, L., Incerti, L., Seida, C., Rebholz, T., Papenmeier, F. (2023). Falsifying the Insufficient Adjustment Model: No Evidence for Unidirectional Adjustment From Anchors. https://osf.io/8cwpy</t>
-  </si>
-  <si>
     <t>https://osf.io/8cwpy</t>
   </si>
   <si>
@@ -789,6 +786,9 @@
   </si>
   <si>
     <t>https://doi.org/10.5281/zenodo.17911973</t>
+  </si>
+  <si>
+    <t>Röseler, L., Incerti, L., Rebholz, T. R., Seida, C., &amp; Papenmeier, F. (2025). Falsifying the insufficient adjustment model: No evidence for unidirectional adjustment from anchors. Meta-Psychology, 9. https://doi.org/10.15626/MP.2024.4137</t>
   </si>
 </sst>
 </file>
@@ -1235,12 +1235,12 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="121.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1254,10 +1254,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -1266,7 +1266,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1274,22 +1274,22 @@
         <v>41</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="D2" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>153</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>154</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>34</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>20</v>
@@ -1303,15 +1303,15 @@
         <v>41</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>10</v>
@@ -1325,15 +1325,15 @@
         <v>11</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>10</v>
@@ -1347,15 +1347,15 @@
         <v>11</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>10</v>
@@ -1369,7 +1369,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>19</v>
@@ -1389,19 +1389,19 @@
         <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="F7" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="G7" s="11" t="s">
         <v>142</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>143</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>10</v>
@@ -1415,17 +1415,17 @@
         <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>20</v>
@@ -1439,15 +1439,15 @@
         <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>10</v>
@@ -1461,10 +1461,10 @@
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>7</v>
@@ -1512,7 +1512,7 @@
         <v>12</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>13</v>
@@ -1542,7 +1542,7 @@
         <v>17</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>18</v>
@@ -1583,7 +1583,7 @@
         <v>25</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>28</v>
@@ -1782,7 +1782,7 @@
         <v>52</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G23" s="7"/>
       <c r="H23" s="2" t="s">
@@ -1942,7 +1942,7 @@
         <v>73</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>74</v>
@@ -1968,7 +1968,7 @@
         <v>78</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>79</v>
@@ -1992,7 +1992,7 @@
         <v>81</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>34</v>
@@ -2018,7 +2018,7 @@
         <v>83</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>84</v>
@@ -2039,19 +2039,19 @@
         <v>21</v>
       </c>
       <c r="C34" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E34" s="4" t="s">
+      <c r="F34" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G34" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>20</v>
@@ -2062,25 +2062,25 @@
         <v>8.5</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="D35" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G35" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H35" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2091,19 +2091,19 @@
         <v>25</v>
       </c>
       <c r="C36" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E36" s="2" t="s">
+      <c r="F36" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="G36" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>20</v>
@@ -2117,19 +2117,19 @@
         <v>32</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E37" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F37" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="G37" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>20</v>
@@ -2143,19 +2143,19 @@
         <v>11</v>
       </c>
       <c r="C38" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E38" s="2" t="s">
+      <c r="F38" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G38" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>10</v>
@@ -2169,17 +2169,17 @@
         <v>32</v>
       </c>
       <c r="C39" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="F39" s="7"/>
       <c r="G39" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>10</v>
@@ -2193,19 +2193,19 @@
         <v>77</v>
       </c>
       <c r="C40" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E40" s="2" t="s">
+      <c r="F40" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="G40" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>109</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>10</v>
@@ -2219,19 +2219,19 @@
         <v>21</v>
       </c>
       <c r="C41" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E41" s="2" t="s">
+      <c r="F41" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="G41" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>20</v>
@@ -2245,19 +2245,19 @@
         <v>41</v>
       </c>
       <c r="C42" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>10</v>
@@ -2268,22 +2268,22 @@
         <v>1</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="D43" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E43" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E43" s="4" t="s">
+      <c r="F43" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="G43" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>10</v>
@@ -2338,36 +2338,35 @@
     <hyperlink ref="G32" r:id="rId45" xr:uid="{5C9D188F-41F0-4255-9A7F-776DC0D7C6B3}"/>
     <hyperlink ref="C33" r:id="rId46" display="https://osf.io/preprints/metaarxiv/ewb2t" xr:uid="{73F38CDC-AE74-42AE-9875-B80E70CAAD04}"/>
     <hyperlink ref="G33" r:id="rId47" xr:uid="{F242B96D-FDF5-4CE7-BDFB-CFE6A00240A0}"/>
-    <hyperlink ref="C34" r:id="rId48" display="https://osf.io/8cwpy" xr:uid="{092A1365-FCB4-41FB-8313-CF735B66A2DD}"/>
-    <hyperlink ref="E34" r:id="rId49" xr:uid="{ECBA28D3-FB1C-4193-901B-41108340BCFD}"/>
-    <hyperlink ref="F34" r:id="rId50" display="https://osf.io/c2ynz" xr:uid="{E93BA08A-3A49-4D35-AC66-D74574AF96C4}"/>
-    <hyperlink ref="F36" r:id="rId51" xr:uid="{97ACEB9A-0C43-4AA2-ACFE-F50A4B6B56F0}"/>
-    <hyperlink ref="C37" r:id="rId52" display="https://doi.org/10.31234/osf.io/2kfh3" xr:uid="{FE4142A2-4633-4F53-8F23-5F50CB46E97C}"/>
-    <hyperlink ref="F37" r:id="rId53" xr:uid="{174B565C-80A9-4205-A2B1-E2DC35E916D7}"/>
-    <hyperlink ref="C38" r:id="rId54" display="https://doi.org/10.31234/osf.io/ntukz" xr:uid="{562912E7-E3CF-4637-A5EC-F5598C18FAED}"/>
-    <hyperlink ref="F38" r:id="rId55" display="https://osf.io/7pw4c/" xr:uid="{E5872E1A-19BD-48E3-BBC5-0325DE4F50E7}"/>
-    <hyperlink ref="C39" r:id="rId56" display="https://doi.org/10.31234/osf.io/wf2tn" xr:uid="{A453771E-19D2-48CD-8D51-59EE29E521DB}"/>
-    <hyperlink ref="C40" r:id="rId57" display="https://doi.org/10.31219/osf.io/2tr6q" xr:uid="{0F998EE8-1C6C-4120-A8A7-D2F043592BCD}"/>
-    <hyperlink ref="F40" r:id="rId58" display="https://osf.io/9qz3d" xr:uid="{4BBBB1B2-2501-4EEF-8BB3-87C7A2170367}"/>
-    <hyperlink ref="C41" r:id="rId59" display="https://doi.org/10.31234/osf.io/hjbwp" xr:uid="{519680D7-CB35-4C47-AB82-99AC96EA8DFE}"/>
-    <hyperlink ref="C42" r:id="rId60" display="https://doi.org/10.31234/osf.io/mt49r" xr:uid="{9EA40F6E-B1C1-4A75-B481-39C90A03E75E}"/>
-    <hyperlink ref="C43" r:id="rId61" display="https://doi.org/10.31234/osf.io/bnsx2" xr:uid="{63D5CDF4-C3ED-4621-886B-026265E45F56}"/>
-    <hyperlink ref="E43" r:id="rId62" xr:uid="{08AABF7C-2FA2-46EF-98CF-56A84170523F}"/>
-    <hyperlink ref="C10" r:id="rId63" display="https://doi.org/10.1007/s41449-025-00460-x" xr:uid="{A0B3F658-F0ED-4C9D-BD5A-8C5E0B28DDAD}"/>
-    <hyperlink ref="E10" r:id="rId64" xr:uid="{86E48510-5694-4822-9C15-811C53298144}"/>
-    <hyperlink ref="F10" r:id="rId65" xr:uid="{F2CF54DC-82BB-4B77-9942-9BF93FA7F0A6}"/>
-    <hyperlink ref="G9" r:id="rId66" xr:uid="{C48C75DC-DB55-4450-A4F7-E9E0C34ECC15}"/>
-    <hyperlink ref="E8" r:id="rId67" xr:uid="{18606C55-07D2-45E4-8557-E96814F20E71}"/>
-    <hyperlink ref="G8" r:id="rId68" xr:uid="{080935E3-AB10-41DA-A9E4-594385CA18FB}"/>
-    <hyperlink ref="E7" r:id="rId69" xr:uid="{CD47EA21-01E5-4F81-861D-1BCF591E3D8D}"/>
-    <hyperlink ref="G7" r:id="rId70" xr:uid="{DB58B12E-C04C-4B6A-99CE-11EF593D3E0F}"/>
-    <hyperlink ref="C36" r:id="rId71" display="https://doi.org/10.31222/osf.io/8psw2" xr:uid="{C0F54102-918A-4578-B027-C78823FD4B7D}"/>
-    <hyperlink ref="G4" r:id="rId72" xr:uid="{5DE4B276-23A0-4D61-A9EA-3B94D7A67DC6}"/>
-    <hyperlink ref="G5" r:id="rId73" xr:uid="{BE4A9D01-B112-43BD-92AC-389201076D3D}"/>
-    <hyperlink ref="E2" r:id="rId74" xr:uid="{BB6A0972-5774-4DF6-9260-A4734EF849A6}"/>
-    <hyperlink ref="G2" r:id="rId75" xr:uid="{99636F1B-E320-48F1-BD31-8C83856946A1}"/>
+    <hyperlink ref="E34" r:id="rId48" xr:uid="{ECBA28D3-FB1C-4193-901B-41108340BCFD}"/>
+    <hyperlink ref="F34" r:id="rId49" display="https://osf.io/c2ynz" xr:uid="{E93BA08A-3A49-4D35-AC66-D74574AF96C4}"/>
+    <hyperlink ref="F36" r:id="rId50" xr:uid="{97ACEB9A-0C43-4AA2-ACFE-F50A4B6B56F0}"/>
+    <hyperlink ref="C37" r:id="rId51" display="https://doi.org/10.31234/osf.io/2kfh3" xr:uid="{FE4142A2-4633-4F53-8F23-5F50CB46E97C}"/>
+    <hyperlink ref="F37" r:id="rId52" xr:uid="{174B565C-80A9-4205-A2B1-E2DC35E916D7}"/>
+    <hyperlink ref="C38" r:id="rId53" display="https://doi.org/10.31234/osf.io/ntukz" xr:uid="{562912E7-E3CF-4637-A5EC-F5598C18FAED}"/>
+    <hyperlink ref="F38" r:id="rId54" display="https://osf.io/7pw4c/" xr:uid="{E5872E1A-19BD-48E3-BBC5-0325DE4F50E7}"/>
+    <hyperlink ref="C39" r:id="rId55" display="https://doi.org/10.31234/osf.io/wf2tn" xr:uid="{A453771E-19D2-48CD-8D51-59EE29E521DB}"/>
+    <hyperlink ref="C40" r:id="rId56" display="https://doi.org/10.31219/osf.io/2tr6q" xr:uid="{0F998EE8-1C6C-4120-A8A7-D2F043592BCD}"/>
+    <hyperlink ref="F40" r:id="rId57" display="https://osf.io/9qz3d" xr:uid="{4BBBB1B2-2501-4EEF-8BB3-87C7A2170367}"/>
+    <hyperlink ref="C41" r:id="rId58" display="https://doi.org/10.31234/osf.io/hjbwp" xr:uid="{519680D7-CB35-4C47-AB82-99AC96EA8DFE}"/>
+    <hyperlink ref="C42" r:id="rId59" display="https://doi.org/10.31234/osf.io/mt49r" xr:uid="{9EA40F6E-B1C1-4A75-B481-39C90A03E75E}"/>
+    <hyperlink ref="C43" r:id="rId60" display="https://doi.org/10.31234/osf.io/bnsx2" xr:uid="{63D5CDF4-C3ED-4621-886B-026265E45F56}"/>
+    <hyperlink ref="E43" r:id="rId61" xr:uid="{08AABF7C-2FA2-46EF-98CF-56A84170523F}"/>
+    <hyperlink ref="C10" r:id="rId62" display="https://doi.org/10.1007/s41449-025-00460-x" xr:uid="{A0B3F658-F0ED-4C9D-BD5A-8C5E0B28DDAD}"/>
+    <hyperlink ref="E10" r:id="rId63" xr:uid="{86E48510-5694-4822-9C15-811C53298144}"/>
+    <hyperlink ref="F10" r:id="rId64" xr:uid="{F2CF54DC-82BB-4B77-9942-9BF93FA7F0A6}"/>
+    <hyperlink ref="G9" r:id="rId65" xr:uid="{C48C75DC-DB55-4450-A4F7-E9E0C34ECC15}"/>
+    <hyperlink ref="E8" r:id="rId66" xr:uid="{18606C55-07D2-45E4-8557-E96814F20E71}"/>
+    <hyperlink ref="G8" r:id="rId67" xr:uid="{080935E3-AB10-41DA-A9E4-594385CA18FB}"/>
+    <hyperlink ref="E7" r:id="rId68" xr:uid="{CD47EA21-01E5-4F81-861D-1BCF591E3D8D}"/>
+    <hyperlink ref="G7" r:id="rId69" xr:uid="{DB58B12E-C04C-4B6A-99CE-11EF593D3E0F}"/>
+    <hyperlink ref="C36" r:id="rId70" display="https://doi.org/10.31222/osf.io/8psw2" xr:uid="{C0F54102-918A-4578-B027-C78823FD4B7D}"/>
+    <hyperlink ref="G4" r:id="rId71" xr:uid="{5DE4B276-23A0-4D61-A9EA-3B94D7A67DC6}"/>
+    <hyperlink ref="G5" r:id="rId72" xr:uid="{BE4A9D01-B112-43BD-92AC-389201076D3D}"/>
+    <hyperlink ref="E2" r:id="rId73" xr:uid="{BB6A0972-5774-4DF6-9260-A4734EF849A6}"/>
+    <hyperlink ref="G2" r:id="rId74" xr:uid="{99636F1B-E320-48F1-BD31-8C83856946A1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId76"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId75"/>
 </worksheet>
 </file>
</xml_diff>